<commit_message>
Fixed some SPARQL that were presented as errors due to typos
</commit_message>
<xml_diff>
--- a/mappings/package_F08/transformation/conceptual_mappings.xlsx
+++ b/mappings/package_F08/transformation/conceptual_mappings.xlsx
@@ -4249,7 +4249,7 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" applyAlignment="1" applyFont="1"/>
   </cellStyleXfs>
-  <cellXfs count="137">
+  <cellXfs count="136">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment readingOrder="0" shrinkToFit="0" vertical="bottom" wrapText="0"/>
     </xf>
@@ -4325,8 +4325,8 @@
     <xf borderId="4" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment vertical="bottom"/>
     </xf>
-    <xf borderId="3" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
+    <xf borderId="3" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
+      <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
     </xf>
     <xf borderId="0" fillId="0" fontId="6" numFmtId="0" xfId="0" applyAlignment="1" applyFont="1">
       <alignment shrinkToFit="0" wrapText="1"/>
@@ -4336,9 +4336,6 @@
     </xf>
     <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment horizontal="center" shrinkToFit="0" vertical="bottom" wrapText="1"/>
-    </xf>
-    <xf borderId="6" fillId="0" fontId="3" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
-      <alignment vertical="bottom"/>
     </xf>
     <xf borderId="6" fillId="0" fontId="1" numFmtId="0" xfId="0" applyAlignment="1" applyBorder="1" applyFont="1">
       <alignment shrinkToFit="0" vertical="bottom" wrapText="1"/>
@@ -8099,25 +8096,25 @@
       <c r="D2" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="E2" s="31" t="s">
+      <c r="E2" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="F2" s="31" t="s">
+      <c r="F2" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="G2" s="31" t="s">
+      <c r="G2" s="30" t="s">
         <v>39</v>
       </c>
       <c r="H2" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="31" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="32" t="s">
+      <c r="J2" s="31" t="s">
         <v>42</v>
       </c>
-      <c r="K2" s="33" t="s">
+      <c r="K2" s="32" t="s">
         <v>43</v>
       </c>
       <c r="L2" s="28"/>
@@ -8137,27 +8134,27 @@
       <c r="Z2" s="28"/>
     </row>
     <row r="3">
-      <c r="A3" s="34" t="s">
+      <c r="A3" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B3" s="35"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="4"/>
       <c r="D3" s="4"/>
-      <c r="E3" s="36" t="s">
+      <c r="E3" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="F3" s="37"/>
-      <c r="G3" s="38" t="s">
+      <c r="F3" s="36"/>
+      <c r="G3" s="37" t="s">
         <v>46</v>
       </c>
-      <c r="H3" s="38" t="s">
+      <c r="H3" s="37" t="s">
         <v>47</v>
       </c>
-      <c r="I3" s="36" t="s">
+      <c r="I3" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="J3" s="36"/>
-      <c r="K3" s="36" t="s">
+      <c r="J3" s="35"/>
+      <c r="K3" s="35" t="s">
         <v>49</v>
       </c>
       <c r="L3" s="28"/>
@@ -8169,25 +8166,25 @@
       <c r="R3" s="28"/>
     </row>
     <row r="4">
-      <c r="A4" s="34" t="s">
+      <c r="A4" s="33" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="35"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="4"/>
       <c r="D4" s="4"/>
-      <c r="E4" s="36" t="s">
+      <c r="E4" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="F4" s="37"/>
-      <c r="G4" s="38" t="s">
+      <c r="F4" s="36"/>
+      <c r="G4" s="37" t="s">
         <v>51</v>
       </c>
-      <c r="H4" s="38" t="s">
+      <c r="H4" s="37" t="s">
         <v>52</v>
       </c>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="39" t="s">
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="38" t="s">
         <v>53</v>
       </c>
       <c r="L4" s="28"/>
@@ -8199,20 +8196,20 @@
       <c r="R4" s="28"/>
     </row>
     <row r="5">
-      <c r="A5" s="34" t="s">
+      <c r="A5" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>55</v>
       </c>
       <c r="C5" s="4"/>
       <c r="D5" s="4"/>
-      <c r="E5" s="36"/>
-      <c r="F5" s="36"/>
-      <c r="G5" s="37"/>
-      <c r="H5" s="37"/>
-      <c r="I5" s="36"/>
-      <c r="J5" s="36"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="36"/>
+      <c r="H5" s="36"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
       <c r="K5" s="7"/>
       <c r="L5" s="28"/>
       <c r="M5" s="28"/>
@@ -8223,20 +8220,20 @@
       <c r="R5" s="28"/>
     </row>
     <row r="6">
-      <c r="A6" s="34" t="s">
+      <c r="A6" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="34" t="s">
         <v>56</v>
       </c>
       <c r="C6" s="4"/>
       <c r="D6" s="4"/>
-      <c r="E6" s="36"/>
-      <c r="F6" s="36"/>
-      <c r="G6" s="37"/>
-      <c r="H6" s="37"/>
-      <c r="I6" s="36"/>
-      <c r="J6" s="36"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="36"/>
+      <c r="H6" s="36"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
       <c r="K6" s="7"/>
       <c r="L6" s="28"/>
       <c r="M6" s="28"/>
@@ -8247,26 +8244,26 @@
       <c r="R6" s="28"/>
     </row>
     <row r="7">
-      <c r="A7" s="40" t="s">
+      <c r="A7" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="B7" s="41" t="s">
+      <c r="B7" s="40" t="s">
         <v>58</v>
       </c>
       <c r="C7" s="4"/>
       <c r="D7" s="4"/>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="35" t="s">
         <v>59</v>
       </c>
-      <c r="F7" s="36"/>
-      <c r="G7" s="36" t="s">
+      <c r="F7" s="35"/>
+      <c r="G7" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="H7" s="36" t="s">
+      <c r="H7" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="I7" s="36"/>
-      <c r="J7" s="36"/>
+      <c r="I7" s="35"/>
+      <c r="J7" s="35"/>
       <c r="K7" s="7"/>
       <c r="L7" s="28"/>
       <c r="M7" s="28"/>
@@ -8277,26 +8274,26 @@
       <c r="R7" s="28"/>
     </row>
     <row r="8">
-      <c r="A8" s="40" t="s">
+      <c r="A8" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="40" t="s">
         <v>58</v>
       </c>
       <c r="C8" s="4"/>
       <c r="D8" s="4"/>
-      <c r="E8" s="42" t="s">
+      <c r="E8" s="41" t="s">
         <v>59</v>
       </c>
-      <c r="F8" s="36"/>
-      <c r="G8" s="36" t="s">
+      <c r="F8" s="35"/>
+      <c r="G8" s="35" t="s">
         <v>62</v>
       </c>
-      <c r="H8" s="36" t="s">
+      <c r="H8" s="35" t="s">
         <v>63</v>
       </c>
-      <c r="I8" s="36"/>
-      <c r="J8" s="36"/>
+      <c r="I8" s="35"/>
+      <c r="J8" s="35"/>
       <c r="K8" s="7"/>
       <c r="L8" s="28"/>
       <c r="M8" s="28"/>
@@ -8307,32 +8304,32 @@
       <c r="R8" s="28"/>
     </row>
     <row r="9">
-      <c r="A9" s="43" t="s">
+      <c r="A9" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="B9" s="44" t="s">
+      <c r="B9" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C9" s="45" t="s">
+      <c r="C9" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="D9" s="45" t="s">
+      <c r="D9" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="E9" s="45" t="s">
+      <c r="E9" s="44" t="s">
         <v>68</v>
       </c>
-      <c r="F9" s="45"/>
-      <c r="G9" s="45" t="s">
+      <c r="F9" s="44"/>
+      <c r="G9" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="H9" s="45" t="s">
+      <c r="H9" s="44" t="s">
         <v>70</v>
       </c>
-      <c r="I9" s="36" t="s">
+      <c r="I9" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="J9" s="36"/>
+      <c r="J9" s="35"/>
       <c r="K9" s="7"/>
       <c r="L9" s="28"/>
       <c r="M9" s="28"/>
@@ -8343,32 +8340,32 @@
       <c r="R9" s="28"/>
     </row>
     <row r="10">
-      <c r="A10" s="43" t="s">
+      <c r="A10" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="B10" s="44" t="s">
+      <c r="B10" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="C10" s="46" t="s">
+      <c r="C10" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="D10" s="46" t="s">
+      <c r="D10" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="E10" s="46" t="s">
+      <c r="E10" s="45" t="s">
         <v>76</v>
       </c>
-      <c r="F10" s="46"/>
-      <c r="G10" s="46" t="s">
+      <c r="F10" s="45"/>
+      <c r="G10" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="H10" s="46" t="s">
+      <c r="H10" s="45" t="s">
         <v>78</v>
       </c>
-      <c r="I10" s="36" t="s">
+      <c r="I10" s="35" t="s">
         <v>79</v>
       </c>
-      <c r="J10" s="36"/>
+      <c r="J10" s="35"/>
       <c r="K10" s="7"/>
       <c r="L10" s="28"/>
       <c r="M10" s="28"/>
@@ -8379,10 +8376,10 @@
       <c r="R10" s="28"/>
     </row>
     <row r="11">
-      <c r="A11" s="47" t="s">
+      <c r="A11" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="B11" s="48" t="s">
+      <c r="B11" s="47" t="s">
         <v>81</v>
       </c>
       <c r="C11" s="4" t="s">
@@ -8391,18 +8388,18 @@
       <c r="D11" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E11" s="36" t="s">
+      <c r="E11" s="35" t="s">
         <v>84</v>
       </c>
-      <c r="F11" s="36"/>
-      <c r="G11" s="36" t="s">
+      <c r="F11" s="35"/>
+      <c r="G11" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="H11" s="36" t="s">
+      <c r="H11" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="I11" s="36"/>
-      <c r="J11" s="36"/>
+      <c r="I11" s="35"/>
+      <c r="J11" s="35"/>
       <c r="K11" s="7"/>
       <c r="L11" s="28"/>
       <c r="M11" s="28"/>
@@ -8413,10 +8410,10 @@
       <c r="R11" s="28"/>
     </row>
     <row r="12">
-      <c r="A12" s="47" t="s">
+      <c r="A12" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="B12" s="48" t="s">
+      <c r="B12" s="47" t="s">
         <v>88</v>
       </c>
       <c r="C12" s="4" t="s">
@@ -8425,18 +8422,18 @@
       <c r="D12" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E12" s="36" t="s">
+      <c r="E12" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="F12" s="36"/>
-      <c r="G12" s="36" t="s">
+      <c r="F12" s="35"/>
+      <c r="G12" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="H12" s="36" t="s">
+      <c r="H12" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="I12" s="36"/>
-      <c r="J12" s="36"/>
+      <c r="I12" s="35"/>
+      <c r="J12" s="35"/>
       <c r="K12" s="7"/>
       <c r="L12" s="28"/>
       <c r="M12" s="28"/>
@@ -8447,32 +8444,32 @@
       <c r="R12" s="28"/>
     </row>
     <row r="13">
-      <c r="A13" s="47" t="s">
+      <c r="A13" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="B13" s="48" t="s">
+      <c r="B13" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="C13" s="49" t="s">
+      <c r="C13" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="D13" s="49" t="s">
+      <c r="D13" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="E13" s="36" t="s">
+      <c r="E13" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="F13" s="36" t="s">
+      <c r="F13" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="G13" s="37" t="s">
+      <c r="G13" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="H13" s="49" t="s">
+      <c r="H13" s="48" t="s">
         <v>100</v>
       </c>
-      <c r="I13" s="36"/>
-      <c r="J13" s="36"/>
+      <c r="I13" s="35"/>
+      <c r="J13" s="35"/>
       <c r="K13" s="7"/>
       <c r="L13" s="28"/>
       <c r="M13" s="28"/>
@@ -8483,10 +8480,10 @@
       <c r="R13" s="28"/>
     </row>
     <row r="14">
-      <c r="A14" s="47" t="s">
+      <c r="A14" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="B14" s="48" t="s">
+      <c r="B14" s="47" t="s">
         <v>102</v>
       </c>
       <c r="C14" s="4" t="s">
@@ -8495,18 +8492,18 @@
       <c r="D14" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E14" s="36" t="s">
+      <c r="E14" s="35" t="s">
         <v>105</v>
       </c>
-      <c r="F14" s="36"/>
-      <c r="G14" s="36" t="s">
+      <c r="F14" s="35"/>
+      <c r="G14" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="H14" s="36" t="s">
+      <c r="H14" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="I14" s="36"/>
-      <c r="J14" s="36"/>
+      <c r="I14" s="35"/>
+      <c r="J14" s="35"/>
       <c r="K14" s="7"/>
       <c r="L14" s="28"/>
       <c r="M14" s="28"/>
@@ -8517,30 +8514,30 @@
       <c r="R14" s="28"/>
     </row>
     <row r="15">
-      <c r="A15" s="43" t="s">
+      <c r="A15" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="B15" s="44" t="s">
+      <c r="B15" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="C15" s="45" t="s">
+      <c r="C15" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="D15" s="45" t="s">
+      <c r="D15" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="E15" s="45" t="s">
+      <c r="E15" s="44" t="s">
         <v>112</v>
       </c>
-      <c r="F15" s="45"/>
-      <c r="G15" s="45" t="s">
+      <c r="F15" s="44"/>
+      <c r="G15" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="H15" s="46" t="s">
+      <c r="H15" s="45" t="s">
         <v>114</v>
       </c>
-      <c r="I15" s="36"/>
-      <c r="J15" s="36"/>
+      <c r="I15" s="35"/>
+      <c r="J15" s="35"/>
       <c r="K15" s="7"/>
       <c r="L15" s="28"/>
       <c r="M15" s="28"/>
@@ -8551,32 +8548,32 @@
       <c r="R15" s="28"/>
     </row>
     <row r="16">
-      <c r="A16" s="47" t="s">
+      <c r="A16" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="B16" s="48" t="s">
+      <c r="B16" s="47" t="s">
         <v>116</v>
       </c>
       <c r="C16" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="D16" s="45" t="s">
+      <c r="D16" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="E16" s="36" t="s">
+      <c r="E16" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="F16" s="36"/>
-      <c r="G16" s="37" t="s">
+      <c r="F16" s="35"/>
+      <c r="G16" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="H16" s="49" t="s">
+      <c r="H16" s="48" t="s">
         <v>120</v>
       </c>
-      <c r="I16" s="36" t="s">
+      <c r="I16" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="J16" s="36"/>
+      <c r="J16" s="35"/>
       <c r="K16" s="7"/>
       <c r="L16" s="28"/>
       <c r="M16" s="28"/>
@@ -8587,10 +8584,10 @@
       <c r="R16" s="28"/>
     </row>
     <row r="17">
-      <c r="A17" s="47" t="s">
+      <c r="A17" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="B17" s="48" t="s">
+      <c r="B17" s="47" t="s">
         <v>122</v>
       </c>
       <c r="C17" s="4" t="s">
@@ -8599,18 +8596,18 @@
       <c r="D17" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E17" s="36" t="s">
+      <c r="E17" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="F17" s="36"/>
-      <c r="G17" s="37" t="s">
+      <c r="F17" s="35"/>
+      <c r="G17" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="H17" s="50" t="s">
+      <c r="H17" s="49" t="s">
         <v>126</v>
       </c>
-      <c r="I17" s="36"/>
-      <c r="J17" s="36"/>
+      <c r="I17" s="35"/>
+      <c r="J17" s="35"/>
       <c r="K17" s="7"/>
       <c r="L17" s="28"/>
       <c r="M17" s="28"/>
@@ -8621,10 +8618,10 @@
       <c r="R17" s="28"/>
     </row>
     <row r="18">
-      <c r="A18" s="47" t="s">
+      <c r="A18" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="B18" s="48" t="s">
+      <c r="B18" s="47" t="s">
         <v>128</v>
       </c>
       <c r="C18" s="4" t="s">
@@ -8633,18 +8630,18 @@
       <c r="D18" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E18" s="36" t="s">
+      <c r="E18" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="F18" s="36"/>
-      <c r="G18" s="37" t="s">
+      <c r="F18" s="35"/>
+      <c r="G18" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="H18" s="49" t="s">
+      <c r="H18" s="48" t="s">
         <v>133</v>
       </c>
-      <c r="I18" s="36"/>
-      <c r="J18" s="36"/>
+      <c r="I18" s="35"/>
+      <c r="J18" s="35"/>
       <c r="K18" s="7"/>
       <c r="L18" s="28"/>
       <c r="M18" s="28"/>
@@ -8655,10 +8652,10 @@
       <c r="R18" s="28"/>
     </row>
     <row r="19">
-      <c r="A19" s="47" t="s">
+      <c r="A19" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="B19" s="48" t="s">
+      <c r="B19" s="47" t="s">
         <v>135</v>
       </c>
       <c r="C19" s="4" t="s">
@@ -8667,18 +8664,18 @@
       <c r="D19" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="E19" s="36" t="s">
+      <c r="E19" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="F19" s="36"/>
-      <c r="G19" s="37" t="s">
+      <c r="F19" s="35"/>
+      <c r="G19" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="H19" s="49" t="s">
+      <c r="H19" s="48" t="s">
         <v>139</v>
       </c>
-      <c r="I19" s="36"/>
-      <c r="J19" s="36"/>
+      <c r="I19" s="35"/>
+      <c r="J19" s="35"/>
       <c r="K19" s="7"/>
       <c r="L19" s="28"/>
       <c r="M19" s="28"/>
@@ -8689,20 +8686,20 @@
       <c r="R19" s="28"/>
     </row>
     <row r="20">
-      <c r="A20" s="47" t="s">
+      <c r="A20" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="B20" s="48" t="s">
+      <c r="B20" s="47" t="s">
         <v>141</v>
       </c>
       <c r="C20" s="4"/>
       <c r="D20" s="4"/>
-      <c r="E20" s="36"/>
-      <c r="F20" s="36"/>
-      <c r="G20" s="36"/>
-      <c r="H20" s="36"/>
-      <c r="I20" s="36"/>
-      <c r="J20" s="36"/>
+      <c r="E20" s="35"/>
+      <c r="F20" s="35"/>
+      <c r="G20" s="35"/>
+      <c r="H20" s="35"/>
+      <c r="I20" s="35"/>
+      <c r="J20" s="35"/>
       <c r="K20" s="7"/>
       <c r="L20" s="28"/>
       <c r="M20" s="28"/>
@@ -8713,30 +8710,30 @@
       <c r="R20" s="28"/>
     </row>
     <row r="21">
-      <c r="A21" s="51" t="s">
+      <c r="A21" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="B21" s="52" t="s">
+      <c r="B21" s="51" t="s">
         <v>143</v>
       </c>
-      <c r="C21" s="45" t="s">
+      <c r="C21" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="D21" s="45" t="s">
+      <c r="D21" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="E21" s="45" t="s">
+      <c r="E21" s="44" t="s">
         <v>146</v>
       </c>
-      <c r="F21" s="45"/>
-      <c r="G21" s="46" t="s">
+      <c r="F21" s="44"/>
+      <c r="G21" s="45" t="s">
         <v>132</v>
       </c>
-      <c r="H21" s="46" t="s">
+      <c r="H21" s="45" t="s">
         <v>147</v>
       </c>
-      <c r="I21" s="36"/>
-      <c r="J21" s="36"/>
+      <c r="I21" s="35"/>
+      <c r="J21" s="35"/>
       <c r="K21" s="7"/>
       <c r="L21" s="28"/>
       <c r="M21" s="28"/>
@@ -8747,10 +8744,10 @@
       <c r="R21" s="28"/>
     </row>
     <row r="22">
-      <c r="A22" s="53" t="s">
+      <c r="A22" s="52" t="s">
         <v>148</v>
       </c>
-      <c r="B22" s="54" t="s">
+      <c r="B22" s="53" t="s">
         <v>149</v>
       </c>
       <c r="C22" s="4" t="s">
@@ -8759,18 +8756,18 @@
       <c r="D22" s="4" t="s">
         <v>151</v>
       </c>
-      <c r="E22" s="36" t="s">
+      <c r="E22" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="F22" s="36"/>
-      <c r="G22" s="36" t="s">
+      <c r="F22" s="35"/>
+      <c r="G22" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="H22" s="49" t="s">
+      <c r="H22" s="48" t="s">
         <v>154</v>
       </c>
-      <c r="I22" s="36"/>
-      <c r="J22" s="36"/>
+      <c r="I22" s="35"/>
+      <c r="J22" s="35"/>
       <c r="K22" s="7"/>
       <c r="L22" s="28"/>
       <c r="M22" s="28"/>
@@ -8781,103 +8778,103 @@
       <c r="R22" s="28"/>
     </row>
     <row r="23">
-      <c r="A23" s="34" t="s">
+      <c r="A23" s="33" t="s">
         <v>54</v>
       </c>
-      <c r="B23" s="35" t="s">
+      <c r="B23" s="34" t="s">
         <v>56</v>
       </c>
       <c r="C23" s="4"/>
       <c r="D23" s="4"/>
-      <c r="E23" s="36"/>
-      <c r="F23" s="36"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
+      <c r="E23" s="35"/>
+      <c r="F23" s="35"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="35"/>
+      <c r="J23" s="35"/>
       <c r="K23" s="7"/>
-      <c r="L23" s="55"/>
-      <c r="M23" s="55"/>
-      <c r="N23" s="55"/>
-      <c r="O23" s="55"/>
-      <c r="P23" s="55"/>
-      <c r="Q23" s="55"/>
-      <c r="R23" s="55"/>
-      <c r="S23" s="56"/>
-      <c r="T23" s="56"/>
-      <c r="U23" s="56"/>
-      <c r="V23" s="56"/>
-      <c r="W23" s="56"/>
-      <c r="X23" s="56"/>
-      <c r="Y23" s="56"/>
-      <c r="Z23" s="56"/>
+      <c r="L23" s="54"/>
+      <c r="M23" s="54"/>
+      <c r="N23" s="54"/>
+      <c r="O23" s="54"/>
+      <c r="P23" s="54"/>
+      <c r="Q23" s="54"/>
+      <c r="R23" s="54"/>
+      <c r="S23" s="55"/>
+      <c r="T23" s="55"/>
+      <c r="U23" s="55"/>
+      <c r="V23" s="55"/>
+      <c r="W23" s="55"/>
+      <c r="X23" s="55"/>
+      <c r="Y23" s="55"/>
+      <c r="Z23" s="55"/>
     </row>
     <row r="24">
-      <c r="A24" s="40" t="s">
+      <c r="A24" s="39" t="s">
         <v>57</v>
       </c>
-      <c r="B24" s="41" t="s">
+      <c r="B24" s="40" t="s">
         <v>58</v>
       </c>
       <c r="C24" s="4"/>
       <c r="D24" s="4"/>
-      <c r="E24" s="42" t="s">
+      <c r="E24" s="41" t="s">
         <v>155</v>
       </c>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36" t="s">
+      <c r="F24" s="35"/>
+      <c r="G24" s="35" t="s">
         <v>60</v>
       </c>
-      <c r="H24" s="36" t="s">
+      <c r="H24" s="35" t="s">
         <v>61</v>
       </c>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
+      <c r="I24" s="35"/>
+      <c r="J24" s="35"/>
       <c r="K24" s="7"/>
-      <c r="L24" s="55"/>
-      <c r="M24" s="55"/>
-      <c r="N24" s="55"/>
-      <c r="O24" s="55"/>
-      <c r="P24" s="55"/>
-      <c r="Q24" s="55"/>
-      <c r="R24" s="55"/>
-      <c r="S24" s="56"/>
-      <c r="T24" s="56"/>
-      <c r="U24" s="56"/>
-      <c r="V24" s="56"/>
-      <c r="W24" s="56"/>
-      <c r="X24" s="56"/>
-      <c r="Y24" s="56"/>
-      <c r="Z24" s="56"/>
+      <c r="L24" s="54"/>
+      <c r="M24" s="54"/>
+      <c r="N24" s="54"/>
+      <c r="O24" s="54"/>
+      <c r="P24" s="54"/>
+      <c r="Q24" s="54"/>
+      <c r="R24" s="54"/>
+      <c r="S24" s="55"/>
+      <c r="T24" s="55"/>
+      <c r="U24" s="55"/>
+      <c r="V24" s="55"/>
+      <c r="W24" s="55"/>
+      <c r="X24" s="55"/>
+      <c r="Y24" s="55"/>
+      <c r="Z24" s="55"/>
     </row>
     <row r="25">
-      <c r="A25" s="43" t="s">
+      <c r="A25" s="42" t="s">
         <v>64</v>
       </c>
-      <c r="B25" s="44" t="s">
+      <c r="B25" s="43" t="s">
         <v>65</v>
       </c>
-      <c r="C25" s="45" t="s">
+      <c r="C25" s="44" t="s">
         <v>66</v>
       </c>
-      <c r="D25" s="45" t="s">
+      <c r="D25" s="44" t="s">
         <v>67</v>
       </c>
-      <c r="E25" s="45" t="s">
+      <c r="E25" s="44" t="s">
         <v>156</v>
       </c>
-      <c r="F25" s="45"/>
-      <c r="G25" s="45" t="s">
+      <c r="F25" s="44"/>
+      <c r="G25" s="44" t="s">
         <v>69</v>
       </c>
-      <c r="H25" s="45" t="s">
+      <c r="H25" s="44" t="s">
         <v>157</v>
       </c>
-      <c r="I25" s="46" t="s">
+      <c r="I25" s="45" t="s">
         <v>71</v>
       </c>
-      <c r="J25" s="46"/>
-      <c r="K25" s="57"/>
+      <c r="J25" s="45"/>
+      <c r="K25" s="56"/>
       <c r="L25" s="28"/>
       <c r="M25" s="28"/>
       <c r="N25" s="28"/>
@@ -8887,33 +8884,33 @@
       <c r="R25" s="28"/>
     </row>
     <row r="26">
-      <c r="A26" s="43" t="s">
+      <c r="A26" s="42" t="s">
         <v>72</v>
       </c>
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="43" t="s">
         <v>73</v>
       </c>
-      <c r="C26" s="46" t="s">
+      <c r="C26" s="45" t="s">
         <v>74</v>
       </c>
-      <c r="D26" s="46" t="s">
+      <c r="D26" s="45" t="s">
         <v>75</v>
       </c>
-      <c r="E26" s="46" t="s">
+      <c r="E26" s="45" t="s">
         <v>158</v>
       </c>
-      <c r="F26" s="46"/>
-      <c r="G26" s="46" t="s">
+      <c r="F26" s="45"/>
+      <c r="G26" s="45" t="s">
         <v>77</v>
       </c>
-      <c r="H26" s="46" t="s">
+      <c r="H26" s="45" t="s">
         <v>159</v>
       </c>
-      <c r="I26" s="45" t="s">
+      <c r="I26" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="J26" s="45"/>
-      <c r="K26" s="57"/>
+      <c r="J26" s="44"/>
+      <c r="K26" s="56"/>
       <c r="L26" s="28"/>
       <c r="M26" s="28"/>
       <c r="N26" s="28"/>
@@ -8923,10 +8920,10 @@
       <c r="R26" s="28"/>
     </row>
     <row r="27">
-      <c r="A27" s="47" t="s">
+      <c r="A27" s="46" t="s">
         <v>80</v>
       </c>
-      <c r="B27" s="48" t="s">
+      <c r="B27" s="47" t="s">
         <v>81</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -8935,18 +8932,18 @@
       <c r="D27" s="4" t="s">
         <v>83</v>
       </c>
-      <c r="E27" s="36" t="s">
+      <c r="E27" s="35" t="s">
         <v>160</v>
       </c>
-      <c r="F27" s="36"/>
-      <c r="G27" s="36" t="s">
+      <c r="F27" s="35"/>
+      <c r="G27" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="H27" s="36" t="s">
+      <c r="H27" s="35" t="s">
         <v>161</v>
       </c>
-      <c r="I27" s="36"/>
-      <c r="J27" s="36"/>
+      <c r="I27" s="35"/>
+      <c r="J27" s="35"/>
       <c r="K27" s="7"/>
       <c r="L27" s="28"/>
       <c r="M27" s="28"/>
@@ -8957,10 +8954,10 @@
       <c r="R27" s="28"/>
     </row>
     <row r="28">
-      <c r="A28" s="47" t="s">
+      <c r="A28" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="B28" s="48" t="s">
+      <c r="B28" s="47" t="s">
         <v>88</v>
       </c>
       <c r="C28" s="4" t="s">
@@ -8969,18 +8966,18 @@
       <c r="D28" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="E28" s="36" t="s">
+      <c r="E28" s="35" t="s">
         <v>162</v>
       </c>
-      <c r="F28" s="36"/>
-      <c r="G28" s="36" t="s">
+      <c r="F28" s="35"/>
+      <c r="G28" s="35" t="s">
         <v>85</v>
       </c>
-      <c r="H28" s="36" t="s">
+      <c r="H28" s="35" t="s">
         <v>163</v>
       </c>
-      <c r="I28" s="36"/>
-      <c r="J28" s="36"/>
+      <c r="I28" s="35"/>
+      <c r="J28" s="35"/>
       <c r="K28" s="7"/>
       <c r="L28" s="28"/>
       <c r="M28" s="28"/>
@@ -8991,54 +8988,54 @@
       <c r="R28" s="28"/>
     </row>
     <row r="29">
-      <c r="A29" s="47" t="s">
+      <c r="A29" s="46" t="s">
         <v>93</v>
       </c>
-      <c r="B29" s="48" t="s">
+      <c r="B29" s="47" t="s">
         <v>94</v>
       </c>
-      <c r="C29" s="49" t="s">
+      <c r="C29" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="D29" s="49" t="s">
+      <c r="D29" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="E29" s="36" t="s">
+      <c r="E29" s="35" t="s">
         <v>164</v>
       </c>
-      <c r="F29" s="36" t="s">
+      <c r="F29" s="35" t="s">
         <v>165</v>
       </c>
-      <c r="G29" s="37" t="s">
+      <c r="G29" s="36" t="s">
         <v>99</v>
       </c>
-      <c r="H29" s="49" t="s">
+      <c r="H29" s="48" t="s">
         <v>166</v>
       </c>
-      <c r="I29" s="36"/>
-      <c r="J29" s="36"/>
+      <c r="I29" s="35"/>
+      <c r="J29" s="35"/>
       <c r="K29" s="7"/>
-      <c r="L29" s="55"/>
-      <c r="M29" s="55"/>
-      <c r="N29" s="55"/>
-      <c r="O29" s="55"/>
-      <c r="P29" s="55"/>
-      <c r="Q29" s="55"/>
-      <c r="R29" s="55"/>
-      <c r="S29" s="56"/>
-      <c r="T29" s="56"/>
-      <c r="U29" s="56"/>
-      <c r="V29" s="56"/>
-      <c r="W29" s="56"/>
-      <c r="X29" s="56"/>
-      <c r="Y29" s="56"/>
-      <c r="Z29" s="56"/>
+      <c r="L29" s="54"/>
+      <c r="M29" s="54"/>
+      <c r="N29" s="54"/>
+      <c r="O29" s="54"/>
+      <c r="P29" s="54"/>
+      <c r="Q29" s="54"/>
+      <c r="R29" s="54"/>
+      <c r="S29" s="55"/>
+      <c r="T29" s="55"/>
+      <c r="U29" s="55"/>
+      <c r="V29" s="55"/>
+      <c r="W29" s="55"/>
+      <c r="X29" s="55"/>
+      <c r="Y29" s="55"/>
+      <c r="Z29" s="55"/>
     </row>
     <row r="30">
-      <c r="A30" s="47" t="s">
+      <c r="A30" s="46" t="s">
         <v>101</v>
       </c>
-      <c r="B30" s="48" t="s">
+      <c r="B30" s="47" t="s">
         <v>102</v>
       </c>
       <c r="C30" s="4" t="s">
@@ -9047,18 +9044,18 @@
       <c r="D30" s="4" t="s">
         <v>104</v>
       </c>
-      <c r="E30" s="36" t="s">
+      <c r="E30" s="35" t="s">
         <v>167</v>
       </c>
-      <c r="F30" s="36"/>
-      <c r="G30" s="36" t="s">
+      <c r="F30" s="35"/>
+      <c r="G30" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="H30" s="36" t="s">
+      <c r="H30" s="35" t="s">
         <v>168</v>
       </c>
-      <c r="I30" s="36"/>
-      <c r="J30" s="36"/>
+      <c r="I30" s="35"/>
+      <c r="J30" s="35"/>
       <c r="K30" s="7"/>
       <c r="L30" s="28"/>
       <c r="M30" s="28"/>
@@ -9069,31 +9066,31 @@
       <c r="R30" s="28"/>
     </row>
     <row r="31">
-      <c r="A31" s="43" t="s">
+      <c r="A31" s="42" t="s">
         <v>108</v>
       </c>
-      <c r="B31" s="44" t="s">
+      <c r="B31" s="43" t="s">
         <v>109</v>
       </c>
-      <c r="C31" s="45" t="s">
+      <c r="C31" s="44" t="s">
         <v>110</v>
       </c>
-      <c r="D31" s="45" t="s">
+      <c r="D31" s="44" t="s">
         <v>111</v>
       </c>
-      <c r="E31" s="45" t="s">
+      <c r="E31" s="44" t="s">
         <v>169</v>
       </c>
-      <c r="F31" s="45"/>
-      <c r="G31" s="45" t="s">
+      <c r="F31" s="44"/>
+      <c r="G31" s="44" t="s">
         <v>113</v>
       </c>
-      <c r="H31" s="45" t="s">
+      <c r="H31" s="44" t="s">
         <v>170</v>
       </c>
-      <c r="I31" s="45"/>
-      <c r="J31" s="45"/>
-      <c r="K31" s="57"/>
+      <c r="I31" s="44"/>
+      <c r="J31" s="44"/>
+      <c r="K31" s="56"/>
       <c r="L31" s="28"/>
       <c r="M31" s="28"/>
       <c r="N31" s="28"/>
@@ -9103,10 +9100,10 @@
       <c r="R31" s="28"/>
     </row>
     <row r="32">
-      <c r="A32" s="47" t="s">
+      <c r="A32" s="46" t="s">
         <v>115</v>
       </c>
-      <c r="B32" s="48" t="s">
+      <c r="B32" s="47" t="s">
         <v>116</v>
       </c>
       <c r="C32" s="4" t="s">
@@ -9115,20 +9112,20 @@
       <c r="D32" s="4" t="s">
         <v>171</v>
       </c>
-      <c r="E32" s="36" t="s">
+      <c r="E32" s="35" t="s">
         <v>172</v>
       </c>
-      <c r="F32" s="36"/>
-      <c r="G32" s="37" t="s">
+      <c r="F32" s="35"/>
+      <c r="G32" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="H32" s="49" t="s">
+      <c r="H32" s="48" t="s">
         <v>173</v>
       </c>
-      <c r="I32" s="36" t="s">
+      <c r="I32" s="35" t="s">
         <v>71</v>
       </c>
-      <c r="J32" s="36"/>
+      <c r="J32" s="35"/>
       <c r="K32" s="7"/>
       <c r="L32" s="28"/>
       <c r="M32" s="28"/>
@@ -9139,10 +9136,10 @@
       <c r="R32" s="28"/>
     </row>
     <row r="33">
-      <c r="A33" s="47" t="s">
+      <c r="A33" s="46" t="s">
         <v>121</v>
       </c>
-      <c r="B33" s="48" t="s">
+      <c r="B33" s="47" t="s">
         <v>122</v>
       </c>
       <c r="C33" s="4" t="s">
@@ -9151,18 +9148,18 @@
       <c r="D33" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="E33" s="36" t="s">
+      <c r="E33" s="35" t="s">
         <v>174</v>
       </c>
-      <c r="F33" s="36"/>
-      <c r="G33" s="37" t="s">
+      <c r="F33" s="35"/>
+      <c r="G33" s="36" t="s">
         <v>119</v>
       </c>
-      <c r="H33" s="50" t="s">
+      <c r="H33" s="49" t="s">
         <v>175</v>
       </c>
-      <c r="I33" s="36"/>
-      <c r="J33" s="36"/>
+      <c r="I33" s="35"/>
+      <c r="J33" s="35"/>
       <c r="K33" s="7"/>
       <c r="L33" s="28"/>
       <c r="M33" s="28"/>
@@ -9173,10 +9170,10 @@
       <c r="R33" s="28"/>
     </row>
     <row r="34">
-      <c r="A34" s="47" t="s">
+      <c r="A34" s="46" t="s">
         <v>127</v>
       </c>
-      <c r="B34" s="48" t="s">
+      <c r="B34" s="47" t="s">
         <v>128</v>
       </c>
       <c r="C34" s="4" t="s">
@@ -9185,18 +9182,18 @@
       <c r="D34" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="E34" s="36" t="s">
+      <c r="E34" s="35" t="s">
         <v>176</v>
       </c>
-      <c r="F34" s="36"/>
-      <c r="G34" s="37" t="s">
+      <c r="F34" s="35"/>
+      <c r="G34" s="36" t="s">
         <v>132</v>
       </c>
-      <c r="H34" s="49" t="s">
+      <c r="H34" s="48" t="s">
         <v>177</v>
       </c>
-      <c r="I34" s="36"/>
-      <c r="J34" s="36"/>
+      <c r="I34" s="35"/>
+      <c r="J34" s="35"/>
       <c r="K34" s="7"/>
       <c r="L34" s="28"/>
       <c r="M34" s="28"/>
@@ -9207,10 +9204,10 @@
       <c r="R34" s="28"/>
     </row>
     <row r="35">
-      <c r="A35" s="47" t="s">
+      <c r="A35" s="46" t="s">
         <v>134</v>
       </c>
-      <c r="B35" s="48" t="s">
+      <c r="B35" s="47" t="s">
         <v>135</v>
       </c>
       <c r="C35" s="4" t="s">
@@ -9219,50 +9216,50 @@
       <c r="D35" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="E35" s="36" t="s">
+      <c r="E35" s="35" t="s">
         <v>178</v>
       </c>
-      <c r="F35" s="36"/>
-      <c r="G35" s="58" t="s">
+      <c r="F35" s="35"/>
+      <c r="G35" s="57" t="s">
         <v>119</v>
       </c>
-      <c r="H35" s="59" t="s">
+      <c r="H35" s="58" t="s">
         <v>179</v>
       </c>
-      <c r="I35" s="36"/>
-      <c r="J35" s="36"/>
+      <c r="I35" s="35"/>
+      <c r="J35" s="35"/>
       <c r="K35" s="7"/>
-      <c r="L35" s="55"/>
-      <c r="M35" s="55"/>
-      <c r="N35" s="55"/>
-      <c r="O35" s="55"/>
-      <c r="P35" s="55"/>
-      <c r="Q35" s="55"/>
-      <c r="R35" s="55"/>
-      <c r="S35" s="56"/>
-      <c r="T35" s="56"/>
-      <c r="U35" s="56"/>
-      <c r="V35" s="56"/>
-      <c r="W35" s="56"/>
-      <c r="X35" s="56"/>
-      <c r="Y35" s="56"/>
-      <c r="Z35" s="56"/>
+      <c r="L35" s="54"/>
+      <c r="M35" s="54"/>
+      <c r="N35" s="54"/>
+      <c r="O35" s="54"/>
+      <c r="P35" s="54"/>
+      <c r="Q35" s="54"/>
+      <c r="R35" s="54"/>
+      <c r="S35" s="55"/>
+      <c r="T35" s="55"/>
+      <c r="U35" s="55"/>
+      <c r="V35" s="55"/>
+      <c r="W35" s="55"/>
+      <c r="X35" s="55"/>
+      <c r="Y35" s="55"/>
+      <c r="Z35" s="55"/>
     </row>
     <row r="36">
-      <c r="A36" s="47" t="s">
+      <c r="A36" s="46" t="s">
         <v>140</v>
       </c>
-      <c r="B36" s="48" t="s">
+      <c r="B36" s="47" t="s">
         <v>141</v>
       </c>
       <c r="C36" s="4"/>
       <c r="D36" s="4"/>
-      <c r="E36" s="36"/>
-      <c r="F36" s="36"/>
+      <c r="E36" s="35"/>
+      <c r="F36" s="35"/>
       <c r="G36" s="4"/>
       <c r="H36" s="4"/>
-      <c r="I36" s="39"/>
-      <c r="J36" s="39"/>
+      <c r="I36" s="38"/>
+      <c r="J36" s="38"/>
       <c r="K36" s="7"/>
       <c r="L36" s="28"/>
       <c r="M36" s="28"/>
@@ -9273,31 +9270,31 @@
       <c r="R36" s="28"/>
     </row>
     <row r="37">
-      <c r="A37" s="51" t="s">
+      <c r="A37" s="50" t="s">
         <v>142</v>
       </c>
-      <c r="B37" s="60" t="s">
+      <c r="B37" s="59" t="s">
         <v>143</v>
       </c>
-      <c r="C37" s="61" t="s">
+      <c r="C37" s="60" t="s">
         <v>144</v>
       </c>
-      <c r="D37" s="61" t="s">
+      <c r="D37" s="60" t="s">
         <v>145</v>
       </c>
-      <c r="E37" s="61" t="s">
+      <c r="E37" s="60" t="s">
         <v>180</v>
       </c>
-      <c r="F37" s="61"/>
-      <c r="G37" s="62" t="s">
+      <c r="F37" s="60"/>
+      <c r="G37" s="61" t="s">
         <v>132</v>
       </c>
-      <c r="H37" s="62" t="s">
+      <c r="H37" s="61" t="s">
         <v>181</v>
       </c>
-      <c r="I37" s="39"/>
-      <c r="J37" s="61"/>
-      <c r="K37" s="57"/>
+      <c r="I37" s="38"/>
+      <c r="J37" s="60"/>
+      <c r="K37" s="56"/>
       <c r="L37" s="28"/>
       <c r="M37" s="28"/>
       <c r="N37" s="28"/>
@@ -9307,10 +9304,10 @@
       <c r="R37" s="28"/>
     </row>
     <row r="38">
-      <c r="A38" s="53" t="s">
+      <c r="A38" s="52" t="s">
         <v>148</v>
       </c>
-      <c r="B38" s="54" t="s">
+      <c r="B38" s="53" t="s">
         <v>149</v>
       </c>
       <c r="C38" s="7" t="s">
@@ -9319,17 +9316,17 @@
       <c r="D38" s="7" t="s">
         <v>151</v>
       </c>
-      <c r="E38" s="36" t="s">
+      <c r="E38" s="35" t="s">
         <v>182</v>
       </c>
-      <c r="F38" s="36"/>
-      <c r="G38" s="36" t="s">
+      <c r="F38" s="35"/>
+      <c r="G38" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="H38" s="49" t="s">
+      <c r="H38" s="48" t="s">
         <v>183</v>
       </c>
-      <c r="I38" s="39"/>
+      <c r="I38" s="38"/>
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
       <c r="L38" s="28"/>
@@ -9341,10 +9338,10 @@
       <c r="R38" s="28"/>
     </row>
     <row r="39">
-      <c r="A39" s="40" t="s">
+      <c r="A39" s="39" t="s">
         <v>184</v>
       </c>
-      <c r="B39" s="41" t="s">
+      <c r="B39" s="40" t="s">
         <v>185</v>
       </c>
       <c r="C39" s="4"/>
@@ -9353,7 +9350,7 @@
       <c r="F39" s="4"/>
       <c r="G39" s="4"/>
       <c r="H39" s="4"/>
-      <c r="I39" s="39"/>
+      <c r="I39" s="38"/>
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
       <c r="L39" s="28"/>
@@ -9365,67 +9362,67 @@
       <c r="R39" s="28"/>
     </row>
     <row r="40">
-      <c r="A40" s="47" t="s">
+      <c r="A40" s="46" t="s">
         <v>186</v>
       </c>
-      <c r="B40" s="48" t="s">
+      <c r="B40" s="47" t="s">
         <v>187</v>
       </c>
-      <c r="C40" s="37"/>
-      <c r="D40" s="37"/>
-      <c r="E40" s="37" t="s">
+      <c r="C40" s="36"/>
+      <c r="D40" s="36"/>
+      <c r="E40" s="36" t="s">
         <v>188</v>
       </c>
-      <c r="F40" s="45"/>
-      <c r="G40" s="37" t="s">
+      <c r="F40" s="44"/>
+      <c r="G40" s="36" t="s">
         <v>189</v>
       </c>
-      <c r="H40" s="49" t="s">
+      <c r="H40" s="48" t="s">
         <v>190</v>
       </c>
-      <c r="I40" s="39"/>
+      <c r="I40" s="38"/>
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
-      <c r="L40" s="55"/>
-      <c r="M40" s="55"/>
-      <c r="N40" s="55"/>
-      <c r="O40" s="55"/>
-      <c r="P40" s="55"/>
-      <c r="Q40" s="55"/>
-      <c r="R40" s="55"/>
-      <c r="S40" s="56"/>
-      <c r="T40" s="56"/>
-      <c r="U40" s="56"/>
-      <c r="V40" s="56"/>
-      <c r="W40" s="56"/>
-      <c r="X40" s="56"/>
-      <c r="Y40" s="56"/>
-      <c r="Z40" s="56"/>
+      <c r="L40" s="54"/>
+      <c r="M40" s="54"/>
+      <c r="N40" s="54"/>
+      <c r="O40" s="54"/>
+      <c r="P40" s="54"/>
+      <c r="Q40" s="54"/>
+      <c r="R40" s="54"/>
+      <c r="S40" s="55"/>
+      <c r="T40" s="55"/>
+      <c r="U40" s="55"/>
+      <c r="V40" s="55"/>
+      <c r="W40" s="55"/>
+      <c r="X40" s="55"/>
+      <c r="Y40" s="55"/>
+      <c r="Z40" s="55"/>
     </row>
     <row r="41">
-      <c r="A41" s="53" t="s">
+      <c r="A41" s="52" t="s">
         <v>191</v>
       </c>
-      <c r="B41" s="54" t="s">
+      <c r="B41" s="53" t="s">
         <v>192</v>
       </c>
-      <c r="C41" s="49" t="s">
+      <c r="C41" s="48" t="s">
         <v>193</v>
       </c>
-      <c r="D41" s="49" t="s">
+      <c r="D41" s="48" t="s">
         <v>194</v>
       </c>
-      <c r="E41" s="37" t="s">
+      <c r="E41" s="36" t="s">
         <v>195</v>
       </c>
-      <c r="F41" s="37"/>
-      <c r="G41" s="37" t="s">
+      <c r="F41" s="36"/>
+      <c r="G41" s="36" t="s">
         <v>196</v>
       </c>
-      <c r="H41" s="49" t="s">
+      <c r="H41" s="48" t="s">
         <v>197</v>
       </c>
-      <c r="I41" s="39" t="s">
+      <c r="I41" s="38" t="s">
         <v>198</v>
       </c>
       <c r="J41" s="7"/>
@@ -9439,25 +9436,25 @@
       <c r="R41" s="28"/>
     </row>
     <row r="42">
-      <c r="A42" s="43" t="s">
+      <c r="A42" s="42" t="s">
         <v>199</v>
       </c>
-      <c r="B42" s="44" t="s">
+      <c r="B42" s="43" t="s">
         <v>200</v>
       </c>
-      <c r="C42" s="46"/>
-      <c r="D42" s="46"/>
-      <c r="E42" s="46" t="s">
+      <c r="C42" s="45"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45" t="s">
         <v>201</v>
       </c>
-      <c r="F42" s="45"/>
-      <c r="G42" s="36" t="s">
+      <c r="F42" s="44"/>
+      <c r="G42" s="35" t="s">
         <v>202</v>
       </c>
-      <c r="H42" s="36" t="s">
+      <c r="H42" s="35" t="s">
         <v>203</v>
       </c>
-      <c r="I42" s="39"/>
+      <c r="I42" s="38"/>
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
       <c r="L42" s="28"/>
@@ -9469,24 +9466,24 @@
       <c r="R42" s="28"/>
     </row>
     <row r="43">
-      <c r="A43" s="40" t="s">
+      <c r="A43" s="39" t="s">
         <v>204</v>
       </c>
-      <c r="B43" s="41" t="s">
+      <c r="B43" s="40" t="s">
         <v>205</v>
       </c>
       <c r="C43" s="4"/>
       <c r="D43" s="4"/>
-      <c r="E43" s="63" t="s">
+      <c r="E43" s="62" t="s">
         <v>206</v>
       </c>
-      <c r="F43" s="63" t="s">
+      <c r="F43" s="62" t="s">
         <v>207</v>
       </c>
-      <c r="G43" s="63" t="s">
+      <c r="G43" s="62" t="s">
         <v>208</v>
       </c>
-      <c r="H43" s="63" t="s">
+      <c r="H43" s="62" t="s">
         <v>209</v>
       </c>
       <c r="I43" s="7"/>
@@ -9501,24 +9498,24 @@
       <c r="R43" s="28"/>
     </row>
     <row r="44">
-      <c r="A44" s="47" t="s">
+      <c r="A44" s="46" t="s">
         <v>210</v>
       </c>
-      <c r="B44" s="48" t="s">
+      <c r="B44" s="47" t="s">
         <v>211</v>
       </c>
-      <c r="C44" s="49" t="s">
+      <c r="C44" s="48" t="s">
         <v>212</v>
       </c>
-      <c r="D44" s="49"/>
-      <c r="E44" s="49" t="s">
+      <c r="D44" s="48"/>
+      <c r="E44" s="48" t="s">
         <v>213</v>
       </c>
-      <c r="F44" s="49"/>
-      <c r="G44" s="49" t="s">
+      <c r="F44" s="48"/>
+      <c r="G44" s="48" t="s">
         <v>214</v>
       </c>
-      <c r="H44" s="49" t="s">
+      <c r="H44" s="48" t="s">
         <v>215</v>
       </c>
       <c r="I44" s="7"/>
@@ -9533,26 +9530,26 @@
       <c r="R44" s="28"/>
     </row>
     <row r="45">
-      <c r="A45" s="53" t="s">
+      <c r="A45" s="52" t="s">
         <v>216</v>
       </c>
-      <c r="B45" s="54" t="s">
+      <c r="B45" s="53" t="s">
         <v>217</v>
       </c>
-      <c r="C45" s="49" t="s">
+      <c r="C45" s="48" t="s">
         <v>218</v>
       </c>
-      <c r="D45" s="49"/>
-      <c r="E45" s="49" t="s">
+      <c r="D45" s="48"/>
+      <c r="E45" s="48" t="s">
         <v>219</v>
       </c>
-      <c r="F45" s="49" t="s">
+      <c r="F45" s="48" t="s">
         <v>220</v>
       </c>
-      <c r="G45" s="49" t="s">
+      <c r="G45" s="48" t="s">
         <v>221</v>
       </c>
-      <c r="H45" s="49" t="s">
+      <c r="H45" s="48" t="s">
         <v>222</v>
       </c>
       <c r="I45" s="7"/>
@@ -9567,24 +9564,24 @@
       <c r="R45" s="28"/>
     </row>
     <row r="46">
-      <c r="A46" s="47" t="s">
+      <c r="A46" s="46" t="s">
         <v>223</v>
       </c>
-      <c r="B46" s="64" t="s">
+      <c r="B46" s="63" t="s">
         <v>224</v>
       </c>
-      <c r="C46" s="59" t="s">
+      <c r="C46" s="58" t="s">
         <v>212</v>
       </c>
-      <c r="D46" s="59"/>
-      <c r="E46" s="59" t="s">
+      <c r="D46" s="58"/>
+      <c r="E46" s="58" t="s">
         <v>225</v>
       </c>
-      <c r="F46" s="59"/>
-      <c r="G46" s="59" t="s">
+      <c r="F46" s="58"/>
+      <c r="G46" s="58" t="s">
         <v>214</v>
       </c>
-      <c r="H46" s="65" t="s">
+      <c r="H46" s="64" t="s">
         <v>226</v>
       </c>
       <c r="I46" s="7"/>
@@ -9599,26 +9596,26 @@
       <c r="R46" s="28"/>
     </row>
     <row r="47">
-      <c r="A47" s="53" t="s">
+      <c r="A47" s="52" t="s">
         <v>227</v>
       </c>
-      <c r="B47" s="54" t="s">
+      <c r="B47" s="53" t="s">
         <v>228</v>
       </c>
-      <c r="C47" s="49" t="s">
+      <c r="C47" s="48" t="s">
         <v>229</v>
       </c>
-      <c r="D47" s="49"/>
-      <c r="E47" s="42" t="s">
+      <c r="D47" s="48"/>
+      <c r="E47" s="41" t="s">
         <v>219</v>
       </c>
-      <c r="F47" s="49" t="s">
+      <c r="F47" s="48" t="s">
         <v>230</v>
       </c>
-      <c r="G47" s="49" t="s">
+      <c r="G47" s="48" t="s">
         <v>221</v>
       </c>
-      <c r="H47" s="49" t="s">
+      <c r="H47" s="48" t="s">
         <v>231</v>
       </c>
       <c r="I47" s="4"/>
@@ -9633,16 +9630,16 @@
       <c r="R47" s="28"/>
     </row>
     <row r="48">
-      <c r="A48" s="47" t="s">
+      <c r="A48" s="46" t="s">
         <v>232</v>
       </c>
-      <c r="B48" s="48" t="s">
+      <c r="B48" s="47" t="s">
         <v>233</v>
       </c>
-      <c r="C48" s="49"/>
-      <c r="D48" s="49"/>
-      <c r="E48" s="49"/>
-      <c r="F48" s="49"/>
+      <c r="C48" s="48"/>
+      <c r="D48" s="48"/>
+      <c r="E48" s="48"/>
+      <c r="F48" s="48"/>
       <c r="G48" s="4"/>
       <c r="H48" s="4"/>
       <c r="I48" s="4"/>
@@ -9657,10 +9654,10 @@
       <c r="R48" s="28"/>
     </row>
     <row r="49">
-      <c r="A49" s="53" t="s">
+      <c r="A49" s="52" t="s">
         <v>234</v>
       </c>
-      <c r="B49" s="54" t="s">
+      <c r="B49" s="53" t="s">
         <v>235</v>
       </c>
       <c r="C49" s="4" t="s">
@@ -9671,50 +9668,50 @@
         <v>237</v>
       </c>
       <c r="F49" s="4"/>
-      <c r="G49" s="63" t="s">
+      <c r="G49" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="H49" s="63" t="s">
+      <c r="H49" s="62" t="s">
         <v>61</v>
       </c>
       <c r="I49" s="7"/>
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
-      <c r="L49" s="55"/>
-      <c r="M49" s="55"/>
-      <c r="N49" s="55"/>
-      <c r="O49" s="55"/>
-      <c r="P49" s="55"/>
-      <c r="Q49" s="55"/>
-      <c r="R49" s="55"/>
-      <c r="S49" s="56"/>
-      <c r="T49" s="56"/>
-      <c r="U49" s="56"/>
-      <c r="V49" s="56"/>
-      <c r="W49" s="56"/>
-      <c r="X49" s="56"/>
-      <c r="Y49" s="56"/>
-      <c r="Z49" s="56"/>
+      <c r="L49" s="54"/>
+      <c r="M49" s="54"/>
+      <c r="N49" s="54"/>
+      <c r="O49" s="54"/>
+      <c r="P49" s="54"/>
+      <c r="Q49" s="54"/>
+      <c r="R49" s="54"/>
+      <c r="S49" s="55"/>
+      <c r="T49" s="55"/>
+      <c r="U49" s="55"/>
+      <c r="V49" s="55"/>
+      <c r="W49" s="55"/>
+      <c r="X49" s="55"/>
+      <c r="Y49" s="55"/>
+      <c r="Z49" s="55"/>
     </row>
     <row r="50">
-      <c r="A50" s="66" t="s">
+      <c r="A50" s="65" t="s">
         <v>234</v>
       </c>
-      <c r="B50" s="67" t="s">
+      <c r="B50" s="66" t="s">
         <v>235</v>
       </c>
-      <c r="C50" s="68" t="s">
+      <c r="C50" s="67" t="s">
         <v>236</v>
       </c>
-      <c r="D50" s="68"/>
-      <c r="E50" s="69" t="s">
+      <c r="D50" s="67"/>
+      <c r="E50" s="68" t="s">
         <v>237</v>
       </c>
       <c r="F50" s="4"/>
-      <c r="G50" s="63" t="s">
+      <c r="G50" s="62" t="s">
         <v>238</v>
       </c>
-      <c r="H50" s="63" t="s">
+      <c r="H50" s="62" t="s">
         <v>239</v>
       </c>
       <c r="I50" s="7"/>
@@ -9729,10 +9726,10 @@
       <c r="R50" s="28"/>
     </row>
     <row r="51">
-      <c r="A51" s="53" t="s">
+      <c r="A51" s="52" t="s">
         <v>240</v>
       </c>
-      <c r="B51" s="54" t="s">
+      <c r="B51" s="53" t="s">
         <v>241</v>
       </c>
       <c r="C51" s="4" t="s">
@@ -9743,15 +9740,15 @@
         <v>242</v>
       </c>
       <c r="F51" s="4"/>
-      <c r="G51" s="70" t="s">
+      <c r="G51" s="69" t="s">
         <v>60</v>
       </c>
-      <c r="H51" s="70" t="s">
+      <c r="H51" s="69" t="s">
         <v>61</v>
       </c>
       <c r="I51" s="7"/>
       <c r="J51" s="7"/>
-      <c r="K51" s="57"/>
+      <c r="K51" s="56"/>
       <c r="L51" s="28"/>
       <c r="M51" s="28"/>
       <c r="N51" s="28"/>
@@ -9761,10 +9758,10 @@
       <c r="R51" s="28"/>
     </row>
     <row r="52">
-      <c r="A52" s="71" t="s">
+      <c r="A52" s="70" t="s">
         <v>243</v>
       </c>
-      <c r="B52" s="72" t="s">
+      <c r="B52" s="71" t="s">
         <v>65</v>
       </c>
       <c r="C52" s="4" t="s">
@@ -9777,13 +9774,13 @@
         <v>244</v>
       </c>
       <c r="F52" s="4"/>
-      <c r="G52" s="70" t="s">
+      <c r="G52" s="69" t="s">
         <v>69</v>
       </c>
-      <c r="H52" s="73" t="s">
+      <c r="H52" s="72" t="s">
         <v>245</v>
       </c>
-      <c r="I52" s="39" t="s">
+      <c r="I52" s="38" t="s">
         <v>71</v>
       </c>
       <c r="J52" s="7"/>
@@ -9797,29 +9794,29 @@
       <c r="R52" s="28"/>
     </row>
     <row r="53">
-      <c r="A53" s="71" t="s">
+      <c r="A53" s="70" t="s">
         <v>246</v>
       </c>
-      <c r="B53" s="72" t="s">
+      <c r="B53" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="C53" s="49" t="s">
+      <c r="C53" s="48" t="s">
         <v>74</v>
       </c>
-      <c r="D53" s="59" t="s">
+      <c r="D53" s="58" t="s">
         <v>75</v>
       </c>
-      <c r="E53" s="49" t="s">
+      <c r="E53" s="48" t="s">
         <v>247</v>
       </c>
-      <c r="F53" s="49"/>
-      <c r="G53" s="70" t="s">
+      <c r="F53" s="48"/>
+      <c r="G53" s="69" t="s">
         <v>77</v>
       </c>
-      <c r="H53" s="73" t="s">
+      <c r="H53" s="72" t="s">
         <v>248</v>
       </c>
-      <c r="I53" s="39" t="s">
+      <c r="I53" s="38" t="s">
         <v>79</v>
       </c>
       <c r="J53" s="7"/>
@@ -9833,10 +9830,10 @@
       <c r="R53" s="28"/>
     </row>
     <row r="54">
-      <c r="A54" s="71" t="s">
+      <c r="A54" s="70" t="s">
         <v>249</v>
       </c>
-      <c r="B54" s="72" t="s">
+      <c r="B54" s="71" t="s">
         <v>81</v>
       </c>
       <c r="C54" s="7" t="s">
@@ -9849,10 +9846,10 @@
         <v>250</v>
       </c>
       <c r="F54" s="4"/>
-      <c r="G54" s="74" t="s">
+      <c r="G54" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="H54" s="75" t="s">
+      <c r="H54" s="74" t="s">
         <v>251</v>
       </c>
       <c r="I54" s="7"/>
@@ -9867,10 +9864,10 @@
       <c r="R54" s="28"/>
     </row>
     <row r="55">
-      <c r="A55" s="71" t="s">
+      <c r="A55" s="70" t="s">
         <v>252</v>
       </c>
-      <c r="B55" s="72" t="s">
+      <c r="B55" s="71" t="s">
         <v>88</v>
       </c>
       <c r="C55" s="4" t="s">
@@ -9883,10 +9880,10 @@
         <v>253</v>
       </c>
       <c r="F55" s="4"/>
-      <c r="G55" s="74" t="s">
+      <c r="G55" s="73" t="s">
         <v>85</v>
       </c>
-      <c r="H55" s="75" t="s">
+      <c r="H55" s="74" t="s">
         <v>254</v>
       </c>
       <c r="I55" s="7"/>
@@ -9901,28 +9898,28 @@
       <c r="R55" s="28"/>
     </row>
     <row r="56">
-      <c r="A56" s="71" t="s">
+      <c r="A56" s="70" t="s">
         <v>255</v>
       </c>
-      <c r="B56" s="72" t="s">
+      <c r="B56" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="C56" s="49" t="s">
+      <c r="C56" s="48" t="s">
         <v>95</v>
       </c>
-      <c r="D56" s="49" t="s">
+      <c r="D56" s="48" t="s">
         <v>96</v>
       </c>
-      <c r="E56" s="36" t="s">
+      <c r="E56" s="35" t="s">
         <v>256</v>
       </c>
-      <c r="F56" s="36" t="s">
+      <c r="F56" s="35" t="s">
         <v>257</v>
       </c>
-      <c r="G56" s="70" t="s">
+      <c r="G56" s="69" t="s">
         <v>99</v>
       </c>
-      <c r="H56" s="73" t="s">
+      <c r="H56" s="72" t="s">
         <v>258</v>
       </c>
       <c r="I56" s="7"/>
@@ -9937,10 +9934,10 @@
       <c r="R56" s="28"/>
     </row>
     <row r="57">
-      <c r="A57" s="71" t="s">
+      <c r="A57" s="70" t="s">
         <v>259</v>
       </c>
-      <c r="B57" s="72" t="s">
+      <c r="B57" s="71" t="s">
         <v>102</v>
       </c>
       <c r="C57" s="4" t="s">
@@ -9953,10 +9950,10 @@
         <v>260</v>
       </c>
       <c r="F57" s="4"/>
-      <c r="G57" s="70" t="s">
+      <c r="G57" s="69" t="s">
         <v>106</v>
       </c>
-      <c r="H57" s="73" t="s">
+      <c r="H57" s="72" t="s">
         <v>261</v>
       </c>
       <c r="I57" s="7"/>
@@ -9971,10 +9968,10 @@
       <c r="R57" s="28"/>
     </row>
     <row r="58">
-      <c r="A58" s="71" t="s">
+      <c r="A58" s="70" t="s">
         <v>262</v>
       </c>
-      <c r="B58" s="72" t="s">
+      <c r="B58" s="71" t="s">
         <v>109</v>
       </c>
       <c r="C58" s="4" t="s">
@@ -9987,10 +9984,10 @@
         <v>263</v>
       </c>
       <c r="F58" s="4"/>
-      <c r="G58" s="70" t="s">
+      <c r="G58" s="69" t="s">
         <v>113</v>
       </c>
-      <c r="H58" s="73" t="s">
+      <c r="H58" s="72" t="s">
         <v>264</v>
       </c>
       <c r="I58" s="7"/>
@@ -10005,10 +10002,10 @@
       <c r="R58" s="28"/>
     </row>
     <row r="59">
-      <c r="A59" s="71" t="s">
+      <c r="A59" s="70" t="s">
         <v>265</v>
       </c>
-      <c r="B59" s="72" t="s">
+      <c r="B59" s="71" t="s">
         <v>116</v>
       </c>
       <c r="C59" s="4" t="s">
@@ -10021,13 +10018,13 @@
         <v>266</v>
       </c>
       <c r="F59" s="4"/>
-      <c r="G59" s="70" t="s">
+      <c r="G59" s="69" t="s">
         <v>119</v>
       </c>
-      <c r="H59" s="73" t="s">
+      <c r="H59" s="72" t="s">
         <v>267</v>
       </c>
-      <c r="I59" s="39" t="s">
+      <c r="I59" s="38" t="s">
         <v>71</v>
       </c>
       <c r="J59" s="7"/>
@@ -10041,10 +10038,10 @@
       <c r="R59" s="28"/>
     </row>
     <row r="60">
-      <c r="A60" s="71" t="s">
+      <c r="A60" s="70" t="s">
         <v>268</v>
       </c>
-      <c r="B60" s="72" t="s">
+      <c r="B60" s="71" t="s">
         <v>122</v>
       </c>
       <c r="C60" s="7" t="s">
@@ -10057,10 +10054,10 @@
         <v>269</v>
       </c>
       <c r="F60" s="4"/>
-      <c r="G60" s="70" t="s">
+      <c r="G60" s="69" t="s">
         <v>119</v>
       </c>
-      <c r="H60" s="73" t="s">
+      <c r="H60" s="72" t="s">
         <v>270</v>
       </c>
       <c r="I60" s="7"/>
@@ -10075,10 +10072,10 @@
       <c r="R60" s="28"/>
     </row>
     <row r="61">
-      <c r="A61" s="71" t="s">
+      <c r="A61" s="70" t="s">
         <v>271</v>
       </c>
-      <c r="B61" s="72" t="s">
+      <c r="B61" s="71" t="s">
         <v>128</v>
       </c>
       <c r="C61" s="7" t="s">
@@ -10091,10 +10088,10 @@
         <v>272</v>
       </c>
       <c r="F61" s="7"/>
-      <c r="G61" s="70" t="s">
+      <c r="G61" s="69" t="s">
         <v>132</v>
       </c>
-      <c r="H61" s="73" t="s">
+      <c r="H61" s="72" t="s">
         <v>273</v>
       </c>
       <c r="I61" s="7"/>
@@ -10109,10 +10106,10 @@
       <c r="R61" s="28"/>
     </row>
     <row r="62">
-      <c r="A62" s="71" t="s">
+      <c r="A62" s="70" t="s">
         <v>274</v>
       </c>
-      <c r="B62" s="72" t="s">
+      <c r="B62" s="71" t="s">
         <v>135</v>
       </c>
       <c r="C62" s="7" t="s">
@@ -10125,10 +10122,10 @@
         <v>275</v>
       </c>
       <c r="F62" s="7"/>
-      <c r="G62" s="70" t="s">
+      <c r="G62" s="69" t="s">
         <v>119</v>
       </c>
-      <c r="H62" s="73" t="s">
+      <c r="H62" s="72" t="s">
         <v>276</v>
       </c>
       <c r="I62" s="7"/>
@@ -10143,10 +10140,10 @@
       <c r="R62" s="28"/>
     </row>
     <row r="63">
-      <c r="A63" s="71" t="s">
+      <c r="A63" s="70" t="s">
         <v>277</v>
       </c>
-      <c r="B63" s="72" t="s">
+      <c r="B63" s="71" t="s">
         <v>141</v>
       </c>
       <c r="C63" s="4"/>
@@ -10167,31 +10164,31 @@
       <c r="R63" s="28"/>
     </row>
     <row r="64">
-      <c r="A64" s="76" t="s">
+      <c r="A64" s="75" t="s">
         <v>278</v>
       </c>
-      <c r="B64" s="45" t="s">
+      <c r="B64" s="44" t="s">
         <v>143</v>
       </c>
-      <c r="C64" s="45" t="s">
+      <c r="C64" s="44" t="s">
         <v>144</v>
       </c>
-      <c r="D64" s="45" t="s">
+      <c r="D64" s="44" t="s">
         <v>145</v>
       </c>
-      <c r="E64" s="45" t="s">
+      <c r="E64" s="44" t="s">
         <v>279</v>
       </c>
-      <c r="F64" s="77"/>
-      <c r="G64" s="78" t="s">
+      <c r="F64" s="76"/>
+      <c r="G64" s="77" t="s">
         <v>132</v>
       </c>
-      <c r="H64" s="78" t="s">
+      <c r="H64" s="77" t="s">
         <v>280</v>
       </c>
-      <c r="I64" s="57"/>
-      <c r="J64" s="57"/>
-      <c r="K64" s="57"/>
+      <c r="I64" s="56"/>
+      <c r="J64" s="56"/>
+      <c r="K64" s="56"/>
       <c r="L64" s="28"/>
       <c r="M64" s="28"/>
       <c r="N64" s="28"/>
@@ -10201,10 +10198,10 @@
       <c r="R64" s="28"/>
     </row>
     <row r="65">
-      <c r="A65" s="47" t="s">
+      <c r="A65" s="46" t="s">
         <v>281</v>
       </c>
-      <c r="B65" s="48" t="s">
+      <c r="B65" s="47" t="s">
         <v>282</v>
       </c>
       <c r="C65" s="4"/>
@@ -10225,24 +10222,24 @@
       <c r="R65" s="28"/>
     </row>
     <row r="66">
-      <c r="A66" s="53" t="s">
+      <c r="A66" s="52" t="s">
         <v>283</v>
       </c>
-      <c r="B66" s="54" t="s">
+      <c r="B66" s="53" t="s">
         <v>284</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>285</v>
       </c>
       <c r="D66" s="4"/>
-      <c r="E66" s="63" t="s">
+      <c r="E66" s="62" t="s">
         <v>286</v>
       </c>
-      <c r="F66" s="79"/>
-      <c r="G66" s="63" t="s">
+      <c r="F66" s="78"/>
+      <c r="G66" s="62" t="s">
         <v>287</v>
       </c>
-      <c r="H66" s="63" t="s">
+      <c r="H66" s="62" t="s">
         <v>288</v>
       </c>
       <c r="I66" s="7"/>
@@ -10257,24 +10254,24 @@
       <c r="R66" s="28"/>
     </row>
     <row r="67">
-      <c r="A67" s="53" t="s">
+      <c r="A67" s="52" t="s">
         <v>289</v>
       </c>
-      <c r="B67" s="54" t="s">
+      <c r="B67" s="53" t="s">
         <v>290</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>291</v>
       </c>
       <c r="D67" s="4"/>
-      <c r="E67" s="63" t="s">
+      <c r="E67" s="62" t="s">
         <v>292</v>
       </c>
-      <c r="F67" s="79"/>
-      <c r="G67" s="63" t="s">
+      <c r="F67" s="78"/>
+      <c r="G67" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="H67" s="63" t="s">
+      <c r="H67" s="62" t="s">
         <v>61</v>
       </c>
       <c r="I67" s="7"/>
@@ -10289,27 +10286,27 @@
       <c r="R67" s="28"/>
     </row>
     <row r="68">
-      <c r="A68" s="80" t="s">
+      <c r="A68" s="79" t="s">
         <v>289</v>
       </c>
-      <c r="B68" s="81" t="s">
+      <c r="B68" s="80" t="s">
         <v>290</v>
       </c>
       <c r="C68" s="4"/>
       <c r="D68" s="4"/>
-      <c r="E68" s="82" t="s">
+      <c r="E68" s="81" t="s">
         <v>292</v>
       </c>
-      <c r="F68" s="83"/>
-      <c r="G68" s="84" t="s">
+      <c r="F68" s="82"/>
+      <c r="G68" s="83" t="s">
         <v>238</v>
       </c>
-      <c r="H68" s="84" t="s">
+      <c r="H68" s="83" t="s">
         <v>239</v>
       </c>
       <c r="I68" s="7"/>
       <c r="J68" s="7"/>
-      <c r="K68" s="39" t="s">
+      <c r="K68" s="38" t="s">
         <v>293</v>
       </c>
       <c r="L68" s="28"/>
@@ -10321,24 +10318,24 @@
       <c r="R68" s="28"/>
     </row>
     <row r="69">
-      <c r="A69" s="53" t="s">
+      <c r="A69" s="52" t="s">
         <v>294</v>
       </c>
-      <c r="B69" s="54" t="s">
+      <c r="B69" s="53" t="s">
         <v>295</v>
       </c>
       <c r="C69" s="4" t="s">
         <v>291</v>
       </c>
       <c r="D69" s="4"/>
-      <c r="E69" s="63" t="s">
+      <c r="E69" s="62" t="s">
         <v>296</v>
       </c>
-      <c r="F69" s="79"/>
-      <c r="G69" s="63" t="s">
+      <c r="F69" s="78"/>
+      <c r="G69" s="62" t="s">
         <v>60</v>
       </c>
-      <c r="H69" s="63" t="s">
+      <c r="H69" s="62" t="s">
         <v>61</v>
       </c>
       <c r="I69" s="7"/>
@@ -10353,29 +10350,29 @@
       <c r="R69" s="28"/>
     </row>
     <row r="70">
-      <c r="A70" s="71" t="s">
+      <c r="A70" s="70" t="s">
         <v>297</v>
       </c>
-      <c r="B70" s="72" t="s">
+      <c r="B70" s="71" t="s">
         <v>65</v>
       </c>
-      <c r="C70" s="36" t="s">
+      <c r="C70" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="D70" s="36" t="s">
+      <c r="D70" s="35" t="s">
         <v>67</v>
       </c>
-      <c r="E70" s="63" t="s">
+      <c r="E70" s="62" t="s">
         <v>298</v>
       </c>
-      <c r="F70" s="79"/>
-      <c r="G70" s="63" t="s">
+      <c r="F70" s="78"/>
+      <c r="G70" s="62" t="s">
         <v>69</v>
       </c>
-      <c r="H70" s="63" t="s">
+      <c r="H70" s="62" t="s">
         <v>299</v>
       </c>
-      <c r="I70" s="39" t="s">
+      <c r="I70" s="38" t="s">
         <v>71</v>
       </c>
       <c r="J70" s="7"/>
@@ -10389,29 +10386,29 @@
       <c r="R70" s="28"/>
     </row>
     <row r="71">
-      <c r="A71" s="71" t="s">
+      <c r="A71" s="70" t="s">
         <v>300</v>
       </c>
-      <c r="B71" s="72" t="s">
+      <c r="B71" s="71" t="s">
         <v>73</v>
       </c>
-      <c r="C71" s="36" t="s">
+      <c r="C71" s="35" t="s">
         <v>74</v>
       </c>
-      <c r="D71" s="36" t="s">
+      <c r="D71" s="35" t="s">
         <v>75</v>
       </c>
-      <c r="E71" s="63" t="s">
+      <c r="E71" s="62" t="s">
         <v>301</v>
       </c>
-      <c r="F71" s="79"/>
-      <c r="G71" s="63" t="s">
+      <c r="F71" s="78"/>
+      <c r="G71" s="62" t="s">
         <v>77</v>
       </c>
-      <c r="H71" s="63" t="s">
+      <c r="H71" s="62" t="s">
         <v>302</v>
       </c>
-      <c r="I71" s="39" t="s">
+      <c r="I71" s="38" t="s">
         <v>79</v>
       </c>
       <c r="J71" s="7"/>
@@ -10425,26 +10422,26 @@
       <c r="R71" s="28"/>
     </row>
     <row r="72">
-      <c r="A72" s="71" t="s">
+      <c r="A72" s="70" t="s">
         <v>303</v>
       </c>
-      <c r="B72" s="72" t="s">
+      <c r="B72" s="71" t="s">
         <v>81</v>
       </c>
-      <c r="C72" s="39" t="s">
+      <c r="C72" s="38" t="s">
         <v>82</v>
       </c>
-      <c r="D72" s="39" t="s">
+      <c r="D72" s="38" t="s">
         <v>83</v>
       </c>
-      <c r="E72" s="63" t="s">
+      <c r="E72" s="62" t="s">
         <v>304</v>
       </c>
-      <c r="F72" s="83"/>
-      <c r="G72" s="63" t="s">
+      <c r="F72" s="82"/>
+      <c r="G72" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="H72" s="63" t="s">
+      <c r="H72" s="62" t="s">
         <v>305</v>
       </c>
       <c r="I72" s="7"/>
@@ -10459,26 +10456,26 @@
       <c r="R72" s="28"/>
     </row>
     <row r="73">
-      <c r="A73" s="71" t="s">
+      <c r="A73" s="70" t="s">
         <v>306</v>
       </c>
-      <c r="B73" s="72" t="s">
+      <c r="B73" s="71" t="s">
         <v>88</v>
       </c>
-      <c r="C73" s="36" t="s">
+      <c r="C73" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="D73" s="36" t="s">
+      <c r="D73" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="E73" s="63" t="s">
+      <c r="E73" s="62" t="s">
         <v>307</v>
       </c>
-      <c r="F73" s="83"/>
-      <c r="G73" s="63" t="s">
+      <c r="F73" s="82"/>
+      <c r="G73" s="62" t="s">
         <v>85</v>
       </c>
-      <c r="H73" s="85" t="s">
+      <c r="H73" s="84" t="s">
         <v>308</v>
       </c>
       <c r="I73" s="7"/>
@@ -10493,28 +10490,28 @@
       <c r="R73" s="28"/>
     </row>
     <row r="74">
-      <c r="A74" s="71" t="s">
+      <c r="A74" s="70" t="s">
         <v>309</v>
       </c>
-      <c r="B74" s="72" t="s">
+      <c r="B74" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="C74" s="36" t="s">
+      <c r="C74" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="D74" s="36" t="s">
+      <c r="D74" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="E74" s="63" t="s">
+      <c r="E74" s="62" t="s">
         <v>310</v>
       </c>
-      <c r="F74" s="63" t="s">
+      <c r="F74" s="62" t="s">
         <v>311</v>
       </c>
-      <c r="G74" s="63" t="s">
+      <c r="G74" s="62" t="s">
         <v>99</v>
       </c>
-      <c r="H74" s="85" t="s">
+      <c r="H74" s="84" t="s">
         <v>312</v>
       </c>
       <c r="I74" s="7"/>
@@ -10529,26 +10526,26 @@
       <c r="R74" s="28"/>
     </row>
     <row r="75">
-      <c r="A75" s="71" t="s">
+      <c r="A75" s="70" t="s">
         <v>313</v>
       </c>
-      <c r="B75" s="72" t="s">
+      <c r="B75" s="71" t="s">
         <v>102</v>
       </c>
-      <c r="C75" s="36" t="s">
+      <c r="C75" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="D75" s="36" t="s">
+      <c r="D75" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="E75" s="63" t="s">
+      <c r="E75" s="62" t="s">
         <v>314</v>
       </c>
-      <c r="F75" s="79"/>
-      <c r="G75" s="63" t="s">
+      <c r="F75" s="78"/>
+      <c r="G75" s="62" t="s">
         <v>106</v>
       </c>
-      <c r="H75" s="63" t="s">
+      <c r="H75" s="62" t="s">
         <v>315</v>
       </c>
       <c r="I75" s="7"/>
@@ -10563,26 +10560,26 @@
       <c r="R75" s="28"/>
     </row>
     <row r="76">
-      <c r="A76" s="71" t="s">
+      <c r="A76" s="70" t="s">
         <v>316</v>
       </c>
-      <c r="B76" s="72" t="s">
+      <c r="B76" s="71" t="s">
         <v>109</v>
       </c>
-      <c r="C76" s="36" t="s">
+      <c r="C76" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="D76" s="36" t="s">
+      <c r="D76" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="E76" s="63" t="s">
+      <c r="E76" s="62" t="s">
         <v>317</v>
       </c>
-      <c r="F76" s="79"/>
-      <c r="G76" s="63" t="s">
+      <c r="F76" s="78"/>
+      <c r="G76" s="62" t="s">
         <v>113</v>
       </c>
-      <c r="H76" s="85" t="s">
+      <c r="H76" s="84" t="s">
         <v>318</v>
       </c>
       <c r="I76" s="7"/>
@@ -10597,29 +10594,29 @@
       <c r="R76" s="28"/>
     </row>
     <row r="77">
-      <c r="A77" s="71" t="s">
+      <c r="A77" s="70" t="s">
         <v>319</v>
       </c>
-      <c r="B77" s="72" t="s">
+      <c r="B77" s="71" t="s">
         <v>116</v>
       </c>
-      <c r="C77" s="36" t="s">
+      <c r="C77" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="D77" s="36" t="s">
+      <c r="D77" s="35" t="s">
         <v>171</v>
       </c>
-      <c r="E77" s="63" t="s">
+      <c r="E77" s="62" t="s">
         <v>320</v>
       </c>
-      <c r="F77" s="83"/>
-      <c r="G77" s="63" t="s">
+      <c r="F77" s="82"/>
+      <c r="G77" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="H77" s="85" t="s">
+      <c r="H77" s="84" t="s">
         <v>321</v>
       </c>
-      <c r="I77" s="39" t="s">
+      <c r="I77" s="38" t="s">
         <v>71</v>
       </c>
       <c r="J77" s="7"/>
@@ -10633,26 +10630,26 @@
       <c r="R77" s="28"/>
     </row>
     <row r="78">
-      <c r="A78" s="71" t="s">
+      <c r="A78" s="70" t="s">
         <v>322</v>
       </c>
-      <c r="B78" s="72" t="s">
+      <c r="B78" s="71" t="s">
         <v>122</v>
       </c>
-      <c r="C78" s="36" t="s">
+      <c r="C78" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="D78" s="36" t="s">
+      <c r="D78" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="E78" s="63" t="s">
+      <c r="E78" s="62" t="s">
         <v>323</v>
       </c>
-      <c r="F78" s="79"/>
-      <c r="G78" s="63" t="s">
+      <c r="F78" s="78"/>
+      <c r="G78" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="H78" s="85" t="s">
+      <c r="H78" s="84" t="s">
         <v>324</v>
       </c>
       <c r="I78" s="7"/>
@@ -10667,26 +10664,26 @@
       <c r="R78" s="28"/>
     </row>
     <row r="79">
-      <c r="A79" s="71" t="s">
+      <c r="A79" s="70" t="s">
         <v>325</v>
       </c>
-      <c r="B79" s="72" t="s">
+      <c r="B79" s="71" t="s">
         <v>128</v>
       </c>
-      <c r="C79" s="36" t="s">
+      <c r="C79" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="D79" s="36" t="s">
+      <c r="D79" s="35" t="s">
         <v>130</v>
       </c>
-      <c r="E79" s="63" t="s">
+      <c r="E79" s="62" t="s">
         <v>326</v>
       </c>
-      <c r="F79" s="79"/>
-      <c r="G79" s="63" t="s">
+      <c r="F79" s="78"/>
+      <c r="G79" s="62" t="s">
         <v>132</v>
       </c>
-      <c r="H79" s="63" t="s">
+      <c r="H79" s="62" t="s">
         <v>327</v>
       </c>
       <c r="I79" s="7"/>
@@ -10701,26 +10698,26 @@
       <c r="R79" s="28"/>
     </row>
     <row r="80">
-      <c r="A80" s="71" t="s">
+      <c r="A80" s="70" t="s">
         <v>328</v>
       </c>
-      <c r="B80" s="72" t="s">
+      <c r="B80" s="71" t="s">
         <v>135</v>
       </c>
-      <c r="C80" s="36" t="s">
+      <c r="C80" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="D80" s="36" t="s">
+      <c r="D80" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="E80" s="63" t="s">
+      <c r="E80" s="62" t="s">
         <v>329</v>
       </c>
-      <c r="F80" s="79"/>
-      <c r="G80" s="63" t="s">
+      <c r="F80" s="78"/>
+      <c r="G80" s="62" t="s">
         <v>119</v>
       </c>
-      <c r="H80" s="63" t="s">
+      <c r="H80" s="62" t="s">
         <v>330</v>
       </c>
       <c r="I80" s="7"/>
@@ -10735,18 +10732,18 @@
       <c r="R80" s="28"/>
     </row>
     <row r="81">
-      <c r="A81" s="71" t="s">
+      <c r="A81" s="70" t="s">
         <v>331</v>
       </c>
-      <c r="B81" s="72" t="s">
+      <c r="B81" s="71" t="s">
         <v>141</v>
       </c>
       <c r="C81" s="4"/>
       <c r="D81" s="4"/>
-      <c r="E81" s="63"/>
-      <c r="F81" s="83"/>
-      <c r="G81" s="63"/>
-      <c r="H81" s="63"/>
+      <c r="E81" s="62"/>
+      <c r="F81" s="82"/>
+      <c r="G81" s="62"/>
+      <c r="H81" s="62"/>
       <c r="I81" s="7"/>
       <c r="J81" s="7"/>
       <c r="K81" s="7"/>
@@ -10759,26 +10756,26 @@
       <c r="R81" s="28"/>
     </row>
     <row r="82">
-      <c r="A82" s="86" t="s">
+      <c r="A82" s="85" t="s">
         <v>332</v>
       </c>
-      <c r="B82" s="36" t="s">
+      <c r="B82" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="C82" s="36" t="s">
+      <c r="C82" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="D82" s="36" t="s">
+      <c r="D82" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="E82" s="63" t="s">
+      <c r="E82" s="62" t="s">
         <v>333</v>
       </c>
-      <c r="F82" s="79"/>
-      <c r="G82" s="63" t="s">
+      <c r="F82" s="78"/>
+      <c r="G82" s="62" t="s">
         <v>132</v>
       </c>
-      <c r="H82" s="63" t="s">
+      <c r="H82" s="62" t="s">
         <v>334</v>
       </c>
       <c r="I82" s="7"/>
@@ -10793,24 +10790,24 @@
       <c r="R82" s="28"/>
     </row>
     <row r="83">
-      <c r="A83" s="47" t="s">
+      <c r="A83" s="46" t="s">
         <v>335</v>
       </c>
-      <c r="B83" s="48" t="s">
+      <c r="B83" s="47" t="s">
         <v>336</v>
       </c>
-      <c r="C83" s="49" t="s">
+      <c r="C83" s="48" t="s">
         <v>337</v>
       </c>
-      <c r="D83" s="49"/>
-      <c r="E83" s="49" t="s">
+      <c r="D83" s="48"/>
+      <c r="E83" s="48" t="s">
         <v>338</v>
       </c>
-      <c r="F83" s="59"/>
-      <c r="G83" s="49" t="s">
+      <c r="F83" s="58"/>
+      <c r="G83" s="48" t="s">
         <v>339</v>
       </c>
-      <c r="H83" s="49" t="s">
+      <c r="H83" s="48" t="s">
         <v>340</v>
       </c>
       <c r="I83" s="7"/>
@@ -10825,24 +10822,24 @@
       <c r="R83" s="28"/>
     </row>
     <row r="84">
-      <c r="A84" s="87" t="s">
+      <c r="A84" s="86" t="s">
         <v>335</v>
       </c>
-      <c r="B84" s="88" t="s">
+      <c r="B84" s="87" t="s">
         <v>336</v>
       </c>
-      <c r="C84" s="89" t="s">
+      <c r="C84" s="88" t="s">
         <v>337</v>
       </c>
-      <c r="D84" s="89"/>
-      <c r="E84" s="90" t="s">
+      <c r="D84" s="88"/>
+      <c r="E84" s="89" t="s">
         <v>338</v>
       </c>
-      <c r="F84" s="37"/>
-      <c r="G84" s="89" t="s">
+      <c r="F84" s="36"/>
+      <c r="G84" s="88" t="s">
         <v>341</v>
       </c>
-      <c r="H84" s="89" t="s">
+      <c r="H84" s="88" t="s">
         <v>342</v>
       </c>
       <c r="I84" s="7"/>
@@ -10857,10 +10854,10 @@
       <c r="R84" s="28"/>
     </row>
     <row r="85">
-      <c r="A85" s="40" t="s">
+      <c r="A85" s="39" t="s">
         <v>343</v>
       </c>
-      <c r="B85" s="41" t="s">
+      <c r="B85" s="40" t="s">
         <v>344</v>
       </c>
       <c r="C85" s="4" t="s">
@@ -10869,19 +10866,19 @@
       <c r="D85" s="4" t="s">
         <v>346</v>
       </c>
-      <c r="E85" s="42" t="s">
+      <c r="E85" s="41" t="s">
         <v>347</v>
       </c>
       <c r="F85" s="4"/>
       <c r="G85" s="4" t="s">
         <v>348</v>
       </c>
-      <c r="H85" s="36" t="s">
+      <c r="H85" s="35" t="s">
         <v>349</v>
       </c>
-      <c r="I85" s="39"/>
-      <c r="J85" s="39"/>
-      <c r="K85" s="39" t="s">
+      <c r="I85" s="38"/>
+      <c r="J85" s="38"/>
+      <c r="K85" s="38" t="s">
         <v>350</v>
       </c>
       <c r="L85" s="28"/>
@@ -10893,20 +10890,20 @@
       <c r="R85" s="28"/>
     </row>
     <row r="86">
-      <c r="A86" s="47" t="s">
+      <c r="A86" s="46" t="s">
         <v>351</v>
       </c>
-      <c r="B86" s="48"/>
+      <c r="B86" s="47"/>
       <c r="C86" s="4"/>
       <c r="D86" s="4"/>
-      <c r="E86" s="36" t="s">
+      <c r="E86" s="35" t="s">
         <v>352</v>
       </c>
-      <c r="F86" s="36"/>
-      <c r="G86" s="36" t="s">
+      <c r="F86" s="35"/>
+      <c r="G86" s="35" t="s">
         <v>353</v>
       </c>
-      <c r="H86" s="36" t="s">
+      <c r="H86" s="35" t="s">
         <v>354</v>
       </c>
       <c r="I86" s="7"/>
@@ -10921,10 +10918,10 @@
       <c r="R86" s="28"/>
     </row>
     <row r="87">
-      <c r="A87" s="40" t="s">
+      <c r="A87" s="39" t="s">
         <v>355</v>
       </c>
-      <c r="B87" s="41" t="s">
+      <c r="B87" s="40" t="s">
         <v>356</v>
       </c>
       <c r="C87" s="4" t="s">
@@ -10933,37 +10930,37 @@
       <c r="D87" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="E87" s="91" t="s">
+      <c r="E87" s="90" t="s">
         <v>359</v>
       </c>
       <c r="F87" s="7"/>
       <c r="G87" s="7" t="s">
         <v>360</v>
       </c>
-      <c r="H87" s="39" t="s">
+      <c r="H87" s="38" t="s">
         <v>361</v>
       </c>
-      <c r="I87" s="39"/>
-      <c r="J87" s="39"/>
-      <c r="K87" s="39" t="s">
+      <c r="I87" s="38"/>
+      <c r="J87" s="38"/>
+      <c r="K87" s="38" t="s">
         <v>350</v>
       </c>
     </row>
     <row r="88">
-      <c r="A88" s="47" t="s">
+      <c r="A88" s="46" t="s">
         <v>362</v>
       </c>
-      <c r="B88" s="48"/>
+      <c r="B88" s="47"/>
       <c r="C88" s="4"/>
       <c r="D88" s="4"/>
-      <c r="E88" s="36" t="s">
+      <c r="E88" s="35" t="s">
         <v>363</v>
       </c>
-      <c r="F88" s="36"/>
-      <c r="G88" s="36" t="s">
+      <c r="F88" s="35"/>
+      <c r="G88" s="35" t="s">
         <v>353</v>
       </c>
-      <c r="H88" s="36" t="s">
+      <c r="H88" s="35" t="s">
         <v>364</v>
       </c>
       <c r="I88" s="7"/>
@@ -10971,10 +10968,10 @@
       <c r="K88" s="7"/>
     </row>
     <row r="89">
-      <c r="A89" s="40" t="s">
+      <c r="A89" s="39" t="s">
         <v>365</v>
       </c>
-      <c r="B89" s="41" t="s">
+      <c r="B89" s="40" t="s">
         <v>366</v>
       </c>
       <c r="C89" s="4" t="s">
@@ -10983,46 +10980,46 @@
       <c r="D89" s="4" t="s">
         <v>358</v>
       </c>
-      <c r="E89" s="42" t="s">
+      <c r="E89" s="41" t="s">
         <v>367</v>
       </c>
       <c r="F89" s="4"/>
       <c r="G89" s="4" t="s">
         <v>360</v>
       </c>
-      <c r="H89" s="36" t="s">
+      <c r="H89" s="35" t="s">
         <v>368</v>
       </c>
-      <c r="I89" s="39"/>
-      <c r="J89" s="39"/>
+      <c r="I89" s="38"/>
+      <c r="J89" s="38"/>
       <c r="K89" s="7"/>
     </row>
     <row r="90">
-      <c r="A90" s="47" t="s">
+      <c r="A90" s="46" t="s">
         <v>369</v>
       </c>
-      <c r="B90" s="48"/>
+      <c r="B90" s="47"/>
       <c r="C90" s="4"/>
       <c r="D90" s="4"/>
-      <c r="E90" s="36" t="s">
+      <c r="E90" s="35" t="s">
         <v>370</v>
       </c>
       <c r="F90" s="4"/>
-      <c r="G90" s="36" t="s">
+      <c r="G90" s="35" t="s">
         <v>353</v>
       </c>
-      <c r="H90" s="36" t="s">
+      <c r="H90" s="35" t="s">
         <v>371</v>
       </c>
-      <c r="I90" s="39"/>
-      <c r="J90" s="39"/>
+      <c r="I90" s="38"/>
+      <c r="J90" s="38"/>
       <c r="K90" s="7"/>
     </row>
     <row r="91">
-      <c r="A91" s="34" t="s">
+      <c r="A91" s="33" t="s">
         <v>372</v>
       </c>
-      <c r="B91" s="92" t="s">
+      <c r="B91" s="91" t="s">
         <v>373</v>
       </c>
       <c r="C91" s="7"/>
@@ -11036,27 +11033,27 @@
       <c r="K91" s="7"/>
     </row>
     <row r="92">
-      <c r="A92" s="40" t="s">
+      <c r="A92" s="39" t="s">
         <v>374</v>
       </c>
-      <c r="B92" s="41" t="s">
+      <c r="B92" s="40" t="s">
         <v>375</v>
       </c>
       <c r="C92" s="7"/>
       <c r="D92" s="7"/>
-      <c r="E92" s="39"/>
-      <c r="F92" s="39"/>
-      <c r="G92" s="39"/>
-      <c r="H92" s="39"/>
-      <c r="I92" s="39"/>
-      <c r="J92" s="39"/>
+      <c r="E92" s="38"/>
+      <c r="F92" s="38"/>
+      <c r="G92" s="38"/>
+      <c r="H92" s="38"/>
+      <c r="I92" s="38"/>
+      <c r="J92" s="38"/>
       <c r="K92" s="7"/>
     </row>
     <row r="93">
-      <c r="A93" s="47" t="s">
+      <c r="A93" s="46" t="s">
         <v>376</v>
       </c>
-      <c r="B93" s="48" t="s">
+      <c r="B93" s="47" t="s">
         <v>6</v>
       </c>
       <c r="C93" s="7" t="s">
@@ -11065,56 +11062,56 @@
       <c r="D93" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="E93" s="39" t="s">
+      <c r="E93" s="38" t="s">
         <v>378</v>
       </c>
-      <c r="F93" s="39"/>
-      <c r="G93" s="39" t="s">
+      <c r="F93" s="38"/>
+      <c r="G93" s="38" t="s">
         <v>379</v>
       </c>
-      <c r="H93" s="39" t="s">
+      <c r="H93" s="38" t="s">
         <v>380</v>
       </c>
-      <c r="I93" s="39" t="s">
+      <c r="I93" s="38" t="s">
         <v>71</v>
       </c>
-      <c r="J93" s="39"/>
-      <c r="K93" s="39"/>
+      <c r="J93" s="38"/>
+      <c r="K93" s="38"/>
     </row>
     <row r="94">
-      <c r="A94" s="51" t="s">
+      <c r="A94" s="50" t="s">
         <v>381</v>
       </c>
-      <c r="B94" s="52" t="s">
+      <c r="B94" s="51" t="s">
         <v>382</v>
       </c>
-      <c r="C94" s="46" t="s">
+      <c r="C94" s="45" t="s">
         <v>383</v>
       </c>
-      <c r="D94" s="46" t="s">
+      <c r="D94" s="45" t="s">
         <v>384</v>
       </c>
-      <c r="E94" s="46" t="s">
+      <c r="E94" s="45" t="s">
         <v>385</v>
       </c>
-      <c r="F94" s="46"/>
-      <c r="G94" s="46" t="s">
+      <c r="F94" s="45"/>
+      <c r="G94" s="45" t="s">
         <v>386</v>
       </c>
-      <c r="H94" s="46" t="s">
+      <c r="H94" s="45" t="s">
         <v>387</v>
       </c>
-      <c r="I94" s="61" t="s">
+      <c r="I94" s="60" t="s">
         <v>79</v>
       </c>
-      <c r="J94" s="57"/>
+      <c r="J94" s="56"/>
       <c r="K94" s="7"/>
     </row>
     <row r="95">
-      <c r="A95" s="47" t="s">
+      <c r="A95" s="46" t="s">
         <v>388</v>
       </c>
-      <c r="B95" s="48" t="s">
+      <c r="B95" s="47" t="s">
         <v>389</v>
       </c>
       <c r="C95" s="4" t="s">
@@ -11123,14 +11120,14 @@
       <c r="D95" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="E95" s="36" t="s">
+      <c r="E95" s="35" t="s">
         <v>392</v>
       </c>
-      <c r="F95" s="36"/>
-      <c r="G95" s="36" t="s">
+      <c r="F95" s="35"/>
+      <c r="G95" s="35" t="s">
         <v>393</v>
       </c>
-      <c r="H95" s="63" t="s">
+      <c r="H95" s="62" t="s">
         <v>394</v>
       </c>
       <c r="I95" s="7"/>
@@ -11138,10 +11135,10 @@
       <c r="K95" s="7"/>
     </row>
     <row r="96">
-      <c r="A96" s="53" t="s">
+      <c r="A96" s="52" t="s">
         <v>395</v>
       </c>
-      <c r="B96" s="54" t="s">
+      <c r="B96" s="53" t="s">
         <v>396</v>
       </c>
       <c r="C96" s="4" t="s">
@@ -11150,23 +11147,23 @@
       <c r="D96" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="E96" s="36" t="s">
+      <c r="E96" s="35" t="s">
         <v>399</v>
       </c>
-      <c r="F96" s="36"/>
-      <c r="G96" s="36"/>
-      <c r="H96" s="36"/>
+      <c r="F96" s="35"/>
+      <c r="G96" s="35"/>
+      <c r="H96" s="35"/>
       <c r="I96" s="7"/>
       <c r="J96" s="7"/>
-      <c r="K96" s="39" t="s">
+      <c r="K96" s="38" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="97">
-      <c r="A97" s="47" t="s">
+      <c r="A97" s="46" t="s">
         <v>401</v>
       </c>
-      <c r="B97" s="48" t="s">
+      <c r="B97" s="47" t="s">
         <v>402</v>
       </c>
       <c r="C97" s="4" t="s">
@@ -11175,14 +11172,14 @@
       <c r="D97" s="4" t="s">
         <v>404</v>
       </c>
-      <c r="E97" s="36" t="s">
+      <c r="E97" s="35" t="s">
         <v>405</v>
       </c>
-      <c r="F97" s="36"/>
-      <c r="G97" s="36" t="s">
+      <c r="F97" s="35"/>
+      <c r="G97" s="35" t="s">
         <v>406</v>
       </c>
-      <c r="H97" s="36" t="s">
+      <c r="H97" s="35" t="s">
         <v>407</v>
       </c>
       <c r="I97" s="7"/>
@@ -11190,41 +11187,41 @@
       <c r="K97" s="7"/>
     </row>
     <row r="98">
-      <c r="A98" s="40" t="s">
+      <c r="A98" s="39" t="s">
         <v>408</v>
       </c>
-      <c r="B98" s="41" t="s">
+      <c r="B98" s="40" t="s">
         <v>8</v>
       </c>
       <c r="C98" s="4"/>
       <c r="D98" s="4"/>
-      <c r="E98" s="42" t="s">
+      <c r="E98" s="41" t="s">
         <v>409</v>
       </c>
       <c r="F98" s="4"/>
-      <c r="G98" s="36"/>
-      <c r="H98" s="36"/>
+      <c r="G98" s="35"/>
+      <c r="H98" s="35"/>
       <c r="I98" s="7"/>
       <c r="J98" s="7"/>
       <c r="K98" s="7"/>
     </row>
     <row r="99">
-      <c r="A99" s="93" t="s">
+      <c r="A99" s="92" t="s">
         <v>408</v>
       </c>
-      <c r="B99" s="94" t="s">
+      <c r="B99" s="93" t="s">
         <v>8</v>
       </c>
       <c r="C99" s="4"/>
       <c r="D99" s="4"/>
-      <c r="E99" s="42" t="s">
+      <c r="E99" s="41" t="s">
         <v>409</v>
       </c>
       <c r="F99" s="4"/>
-      <c r="G99" s="63" t="s">
+      <c r="G99" s="62" t="s">
         <v>410</v>
       </c>
-      <c r="H99" s="63" t="s">
+      <c r="H99" s="62" t="s">
         <v>411</v>
       </c>
       <c r="I99" s="7"/>
@@ -11232,10 +11229,10 @@
       <c r="K99" s="7"/>
     </row>
     <row r="100">
-      <c r="A100" s="47" t="s">
+      <c r="A100" s="46" t="s">
         <v>412</v>
       </c>
-      <c r="B100" s="48" t="s">
+      <c r="B100" s="47" t="s">
         <v>413</v>
       </c>
       <c r="C100" s="4"/>
@@ -11249,10 +11246,10 @@
       <c r="K100" s="7"/>
     </row>
     <row r="101">
-      <c r="A101" s="53" t="s">
+      <c r="A101" s="52" t="s">
         <v>414</v>
       </c>
-      <c r="B101" s="54" t="s">
+      <c r="B101" s="53" t="s">
         <v>389</v>
       </c>
       <c r="C101" s="4" t="s">
@@ -11261,14 +11258,14 @@
       <c r="D101" s="4" t="s">
         <v>391</v>
       </c>
-      <c r="E101" s="36" t="s">
+      <c r="E101" s="35" t="s">
         <v>415</v>
       </c>
-      <c r="F101" s="36"/>
-      <c r="G101" s="36" t="s">
+      <c r="F101" s="35"/>
+      <c r="G101" s="35" t="s">
         <v>416</v>
       </c>
-      <c r="H101" s="36" t="s">
+      <c r="H101" s="35" t="s">
         <v>417</v>
       </c>
       <c r="I101" s="7"/>
@@ -11276,10 +11273,10 @@
       <c r="K101" s="7"/>
     </row>
     <row r="102">
-      <c r="A102" s="53" t="s">
+      <c r="A102" s="52" t="s">
         <v>418</v>
       </c>
-      <c r="B102" s="54" t="s">
+      <c r="B102" s="53" t="s">
         <v>396</v>
       </c>
       <c r="C102" s="4" t="s">
@@ -11288,23 +11285,23 @@
       <c r="D102" s="4" t="s">
         <v>398</v>
       </c>
-      <c r="E102" s="36" t="s">
+      <c r="E102" s="35" t="s">
         <v>419</v>
       </c>
-      <c r="F102" s="36"/>
-      <c r="G102" s="36"/>
-      <c r="H102" s="36"/>
+      <c r="F102" s="35"/>
+      <c r="G102" s="35"/>
+      <c r="H102" s="35"/>
       <c r="I102" s="7"/>
       <c r="J102" s="7"/>
-      <c r="K102" s="39" t="s">
+      <c r="K102" s="38" t="s">
         <v>400</v>
       </c>
     </row>
     <row r="103">
-      <c r="A103" s="47" t="s">
+      <c r="A103" s="46" t="s">
         <v>420</v>
       </c>
-      <c r="B103" s="48" t="s">
+      <c r="B103" s="47" t="s">
         <v>421</v>
       </c>
       <c r="C103" s="4"/>
@@ -11318,10 +11315,10 @@
       <c r="K103" s="7"/>
     </row>
     <row r="104">
-      <c r="A104" s="53" t="s">
+      <c r="A104" s="52" t="s">
         <v>422</v>
       </c>
-      <c r="B104" s="54" t="s">
+      <c r="B104" s="53" t="s">
         <v>94</v>
       </c>
       <c r="C104" s="4" t="s">
@@ -11330,16 +11327,16 @@
       <c r="D104" s="4" t="s">
         <v>424</v>
       </c>
-      <c r="E104" s="36" t="s">
+      <c r="E104" s="35" t="s">
         <v>425</v>
       </c>
-      <c r="F104" s="36" t="s">
+      <c r="F104" s="35" t="s">
         <v>426</v>
       </c>
-      <c r="G104" s="37" t="s">
+      <c r="G104" s="36" t="s">
         <v>427</v>
       </c>
-      <c r="H104" s="95" t="s">
+      <c r="H104" s="94" t="s">
         <v>428</v>
       </c>
       <c r="I104" s="7"/>
@@ -11347,97 +11344,97 @@
       <c r="K104" s="7"/>
     </row>
     <row r="105">
-      <c r="A105" s="53" t="s">
+      <c r="A105" s="52" t="s">
         <v>429</v>
       </c>
-      <c r="B105" s="54" t="s">
+      <c r="B105" s="53" t="s">
         <v>430</v>
       </c>
-      <c r="C105" s="49" t="s">
+      <c r="C105" s="48" t="s">
         <v>431</v>
       </c>
-      <c r="D105" s="49" t="s">
+      <c r="D105" s="48" t="s">
         <v>432</v>
       </c>
-      <c r="E105" s="36" t="s">
+      <c r="E105" s="35" t="s">
         <v>433</v>
       </c>
-      <c r="F105" s="36"/>
-      <c r="G105" s="37" t="s">
+      <c r="F105" s="35"/>
+      <c r="G105" s="36" t="s">
         <v>434</v>
       </c>
-      <c r="H105" s="96" t="s">
+      <c r="H105" s="95" t="s">
         <v>435</v>
       </c>
-      <c r="I105" s="39" t="s">
+      <c r="I105" s="38" t="s">
         <v>71</v>
       </c>
       <c r="J105" s="7"/>
       <c r="K105" s="7"/>
     </row>
     <row r="106">
-      <c r="A106" s="47" t="s">
+      <c r="A106" s="46" t="s">
         <v>436</v>
       </c>
-      <c r="B106" s="48" t="s">
+      <c r="B106" s="47" t="s">
         <v>437</v>
       </c>
-      <c r="C106" s="49" t="s">
+      <c r="C106" s="48" t="s">
         <v>438</v>
       </c>
-      <c r="D106" s="59" t="s">
+      <c r="D106" s="58" t="s">
         <v>8</v>
       </c>
-      <c r="E106" s="39" t="s">
+      <c r="E106" s="38" t="s">
         <v>439</v>
       </c>
-      <c r="F106" s="39"/>
-      <c r="G106" s="39" t="s">
+      <c r="F106" s="38"/>
+      <c r="G106" s="38" t="s">
         <v>440</v>
       </c>
-      <c r="H106" s="97" t="s">
+      <c r="H106" s="96" t="s">
         <v>441</v>
       </c>
-      <c r="I106" s="39" t="s">
+      <c r="I106" s="38" t="s">
         <v>71</v>
       </c>
       <c r="J106" s="7"/>
       <c r="K106" s="7"/>
     </row>
     <row r="107">
-      <c r="A107" s="47" t="s">
+      <c r="A107" s="46" t="s">
         <v>436</v>
       </c>
-      <c r="B107" s="48" t="s">
+      <c r="B107" s="47" t="s">
         <v>442</v>
       </c>
-      <c r="C107" s="49" t="s">
+      <c r="C107" s="48" t="s">
         <v>438</v>
       </c>
-      <c r="D107" s="49" t="s">
+      <c r="D107" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="E107" s="42" t="s">
+      <c r="E107" s="41" t="s">
         <v>439</v>
       </c>
-      <c r="F107" s="36"/>
-      <c r="G107" s="36" t="s">
+      <c r="F107" s="35"/>
+      <c r="G107" s="35" t="s">
         <v>440</v>
       </c>
-      <c r="H107" s="98" t="s">
+      <c r="H107" s="97" t="s">
         <v>443</v>
       </c>
-      <c r="I107" s="39" t="s">
+      <c r="I107" s="38" t="s">
         <v>71</v>
       </c>
       <c r="J107" s="7"/>
       <c r="K107" s="7"/>
     </row>
     <row r="108">
-      <c r="A108" s="34" t="s">
+      <c r="A108" s="33" t="s">
         <v>444</v>
       </c>
-      <c r="B108" s="35" t="s">
+      <c r="B108" s="34" t="s">
         <v>445</v>
       </c>
       <c r="C108" s="4"/>
@@ -11451,55 +11448,55 @@
       <c r="K108" s="7"/>
     </row>
     <row r="109">
-      <c r="A109" s="40" t="s">
+      <c r="A109" s="39" t="s">
         <v>446</v>
       </c>
-      <c r="B109" s="41" t="s">
+      <c r="B109" s="40" t="s">
         <v>447</v>
       </c>
-      <c r="C109" s="49" t="s">
+      <c r="C109" s="48" t="s">
         <v>448</v>
       </c>
       <c r="D109" s="7" t="s">
         <v>449</v>
       </c>
-      <c r="E109" s="99" t="s">
+      <c r="E109" s="98" t="s">
         <v>450</v>
       </c>
-      <c r="F109" s="99"/>
-      <c r="G109" s="100" t="s">
+      <c r="F109" s="98"/>
+      <c r="G109" s="99" t="s">
         <v>379</v>
       </c>
-      <c r="H109" s="101" t="s">
+      <c r="H109" s="100" t="s">
         <v>451</v>
       </c>
-      <c r="I109" s="39" t="s">
+      <c r="I109" s="38" t="s">
         <v>71</v>
       </c>
       <c r="J109" s="7"/>
       <c r="K109" s="7"/>
     </row>
     <row r="110">
-      <c r="A110" s="40" t="s">
+      <c r="A110" s="39" t="s">
         <v>452</v>
       </c>
-      <c r="B110" s="41" t="s">
+      <c r="B110" s="40" t="s">
         <v>453</v>
       </c>
-      <c r="C110" s="102" t="s">
+      <c r="C110" s="101" t="s">
         <v>454</v>
       </c>
-      <c r="D110" s="102" t="s">
+      <c r="D110" s="101" t="s">
         <v>455</v>
       </c>
-      <c r="E110" s="103" t="s">
+      <c r="E110" s="102" t="s">
         <v>456</v>
       </c>
-      <c r="F110" s="103"/>
-      <c r="G110" s="36" t="s">
+      <c r="F110" s="102"/>
+      <c r="G110" s="35" t="s">
         <v>457</v>
       </c>
-      <c r="H110" s="104" t="s">
+      <c r="H110" s="103" t="s">
         <v>458</v>
       </c>
       <c r="I110" s="7"/>
@@ -11568,22 +11565,22 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="105" t="s">
+      <c r="A1" s="104" t="s">
         <v>33</v>
       </c>
-      <c r="B1" s="106" t="s">
+      <c r="B1" s="105" t="s">
         <v>34</v>
       </c>
-      <c r="C1" s="106" t="s">
+      <c r="C1" s="105" t="s">
         <v>35</v>
       </c>
-      <c r="D1" s="106" t="s">
+      <c r="D1" s="105" t="s">
         <v>36</v>
       </c>
-      <c r="E1" s="106" t="s">
+      <c r="E1" s="105" t="s">
         <v>37</v>
       </c>
-      <c r="F1" s="106" t="s">
+      <c r="F1" s="105" t="s">
         <v>2</v>
       </c>
     </row>
@@ -11594,16 +11591,16 @@
       <c r="B2" s="4" t="s">
         <v>396</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="38" t="s">
         <v>397</v>
       </c>
-      <c r="D2" s="39" t="s">
+      <c r="D2" s="38" t="s">
         <v>398</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>399</v>
       </c>
-      <c r="F2" s="36" t="s">
+      <c r="F2" s="35" t="s">
         <v>459</v>
       </c>
     </row>
@@ -11611,17 +11608,17 @@
       <c r="A3" s="18" t="s">
         <v>460</v>
       </c>
-      <c r="B3" s="39" t="s">
+      <c r="B3" s="38" t="s">
         <v>461</v>
       </c>
-      <c r="C3" s="59" t="s">
+      <c r="C3" s="58" t="s">
         <v>462</v>
       </c>
-      <c r="D3" s="59"/>
-      <c r="E3" s="36" t="s">
+      <c r="D3" s="58"/>
+      <c r="E3" s="35" t="s">
         <v>463</v>
       </c>
-      <c r="F3" s="36" t="s">
+      <c r="F3" s="35" t="s">
         <v>464</v>
       </c>
     </row>
@@ -11629,17 +11626,17 @@
       <c r="A4" s="18" t="s">
         <v>460</v>
       </c>
-      <c r="B4" s="39" t="s">
+      <c r="B4" s="38" t="s">
         <v>461</v>
       </c>
-      <c r="C4" s="59" t="s">
+      <c r="C4" s="58" t="s">
         <v>462</v>
       </c>
-      <c r="D4" s="59"/>
-      <c r="E4" s="36" t="s">
+      <c r="D4" s="58"/>
+      <c r="E4" s="35" t="s">
         <v>465</v>
       </c>
-      <c r="F4" s="36" t="s">
+      <c r="F4" s="35" t="s">
         <v>466</v>
       </c>
     </row>
@@ -11650,82 +11647,82 @@
       <c r="B5" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="C5" s="39" t="s">
+      <c r="C5" s="38" t="s">
         <v>397</v>
       </c>
-      <c r="D5" s="39" t="s">
+      <c r="D5" s="38" t="s">
         <v>398</v>
       </c>
       <c r="E5" s="4" t="s">
         <v>419</v>
       </c>
-      <c r="F5" s="36" t="s">
+      <c r="F5" s="35" t="s">
         <v>467</v>
       </c>
-      <c r="G5" s="107"/>
-      <c r="H5" s="107"/>
-      <c r="I5" s="107"/>
-      <c r="J5" s="107"/>
-      <c r="K5" s="107"/>
-      <c r="L5" s="107"/>
-      <c r="M5" s="107"/>
-      <c r="N5" s="107"/>
-      <c r="O5" s="107"/>
-      <c r="P5" s="107"/>
-      <c r="Q5" s="107"/>
-      <c r="R5" s="107"/>
-      <c r="S5" s="107"/>
-      <c r="T5" s="107"/>
-      <c r="U5" s="107"/>
-      <c r="V5" s="107"/>
-      <c r="W5" s="107"/>
-      <c r="X5" s="107"/>
-      <c r="Y5" s="107"/>
-      <c r="Z5" s="107"/>
+      <c r="G5" s="106"/>
+      <c r="H5" s="106"/>
+      <c r="I5" s="106"/>
+      <c r="J5" s="106"/>
+      <c r="K5" s="106"/>
+      <c r="L5" s="106"/>
+      <c r="M5" s="106"/>
+      <c r="N5" s="106"/>
+      <c r="O5" s="106"/>
+      <c r="P5" s="106"/>
+      <c r="Q5" s="106"/>
+      <c r="R5" s="106"/>
+      <c r="S5" s="106"/>
+      <c r="T5" s="106"/>
+      <c r="U5" s="106"/>
+      <c r="V5" s="106"/>
+      <c r="W5" s="106"/>
+      <c r="X5" s="106"/>
+      <c r="Y5" s="106"/>
+      <c r="Z5" s="106"/>
     </row>
     <row r="6">
       <c r="A6" s="18" t="s">
         <v>468</v>
       </c>
-      <c r="B6" s="39" t="s">
+      <c r="B6" s="38" t="s">
         <v>469</v>
       </c>
-      <c r="C6" s="59" t="s">
+      <c r="C6" s="58" t="s">
         <v>470</v>
       </c>
-      <c r="D6" s="59" t="s">
+      <c r="D6" s="58" t="s">
         <v>471</v>
       </c>
-      <c r="E6" s="36" t="s">
+      <c r="E6" s="35" t="s">
         <v>472</v>
       </c>
-      <c r="F6" s="36"/>
-      <c r="G6" s="107"/>
-      <c r="H6" s="107"/>
-      <c r="I6" s="107"/>
-      <c r="J6" s="107"/>
-      <c r="K6" s="107"/>
-      <c r="L6" s="107"/>
-      <c r="M6" s="107"/>
-      <c r="N6" s="107"/>
-      <c r="O6" s="107"/>
-      <c r="P6" s="107"/>
-      <c r="Q6" s="107"/>
-      <c r="R6" s="107"/>
-      <c r="S6" s="107"/>
-      <c r="T6" s="107"/>
-      <c r="U6" s="107"/>
-      <c r="V6" s="107"/>
-      <c r="W6" s="107"/>
-      <c r="X6" s="107"/>
-      <c r="Y6" s="107"/>
-      <c r="Z6" s="107"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="106"/>
+      <c r="H6" s="106"/>
+      <c r="I6" s="106"/>
+      <c r="J6" s="106"/>
+      <c r="K6" s="106"/>
+      <c r="L6" s="106"/>
+      <c r="M6" s="106"/>
+      <c r="N6" s="106"/>
+      <c r="O6" s="106"/>
+      <c r="P6" s="106"/>
+      <c r="Q6" s="106"/>
+      <c r="R6" s="106"/>
+      <c r="S6" s="106"/>
+      <c r="T6" s="106"/>
+      <c r="U6" s="106"/>
+      <c r="V6" s="106"/>
+      <c r="W6" s="106"/>
+      <c r="X6" s="106"/>
+      <c r="Y6" s="106"/>
+      <c r="Z6" s="106"/>
     </row>
     <row r="7">
       <c r="A7" s="18" t="s">
         <v>473</v>
       </c>
-      <c r="B7" s="36" t="s">
+      <c r="B7" s="35" t="s">
         <v>474</v>
       </c>
       <c r="C7" s="7" t="s">
@@ -11734,10 +11731,10 @@
       <c r="D7" s="7" t="s">
         <v>476</v>
       </c>
-      <c r="E7" s="36" t="s">
+      <c r="E7" s="35" t="s">
         <v>477</v>
       </c>
-      <c r="F7" s="36" t="s">
+      <c r="F7" s="35" t="s">
         <v>478</v>
       </c>
     </row>
@@ -11748,32 +11745,32 @@
       <c r="B8" s="7" t="s">
         <v>480</v>
       </c>
-      <c r="C8" s="39" t="s">
+      <c r="C8" s="38" t="s">
         <v>481</v>
       </c>
       <c r="D8" s="7"/>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="38" t="s">
         <v>482</v>
       </c>
-      <c r="F8" s="39" t="s">
+      <c r="F8" s="38" t="s">
         <v>483</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="84" t="s">
+      <c r="A9" s="83" t="s">
         <v>484</v>
       </c>
-      <c r="B9" s="84" t="s">
+      <c r="B9" s="83" t="s">
         <v>485</v>
       </c>
-      <c r="C9" s="84" t="s">
+      <c r="C9" s="83" t="s">
         <v>481</v>
       </c>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84" t="s">
+      <c r="D9" s="83"/>
+      <c r="E9" s="83" t="s">
         <v>486</v>
       </c>
-      <c r="F9" s="84" t="s">
+      <c r="F9" s="83" t="s">
         <v>483</v>
       </c>
     </row>
@@ -11781,17 +11778,17 @@
       <c r="A10" s="7" t="s">
         <v>487</v>
       </c>
-      <c r="B10" s="39" t="s">
+      <c r="B10" s="38" t="s">
         <v>488</v>
       </c>
-      <c r="C10" s="108" t="s">
+      <c r="C10" s="107" t="s">
         <v>489</v>
       </c>
       <c r="D10" s="7"/>
-      <c r="E10" s="39" t="s">
+      <c r="E10" s="38" t="s">
         <v>490</v>
       </c>
-      <c r="F10" s="39" t="s">
+      <c r="F10" s="38" t="s">
         <v>491</v>
       </c>
     </row>
@@ -11799,7 +11796,7 @@
       <c r="A11" s="7" t="s">
         <v>492</v>
       </c>
-      <c r="B11" s="39" t="s">
+      <c r="B11" s="38" t="s">
         <v>493</v>
       </c>
       <c r="C11" s="7" t="s">
@@ -11808,30 +11805,30 @@
       <c r="D11" s="7" t="s">
         <v>495</v>
       </c>
-      <c r="E11" s="39" t="s">
+      <c r="E11" s="38" t="s">
         <v>496</v>
       </c>
-      <c r="F11" s="39" t="s">
+      <c r="F11" s="38" t="s">
         <v>497</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" s="83" t="s">
+      <c r="A12" s="82" t="s">
         <v>498</v>
       </c>
-      <c r="B12" s="84" t="s">
+      <c r="B12" s="83" t="s">
         <v>499</v>
       </c>
-      <c r="C12" s="83" t="s">
+      <c r="C12" s="82" t="s">
         <v>500</v>
       </c>
-      <c r="D12" s="83" t="s">
+      <c r="D12" s="82" t="s">
         <v>501</v>
       </c>
-      <c r="E12" s="84" t="s">
+      <c r="E12" s="83" t="s">
         <v>502</v>
       </c>
-      <c r="F12" s="109" t="s">
+      <c r="F12" s="108" t="s">
         <v>503</v>
       </c>
     </row>
@@ -11839,31 +11836,31 @@
       <c r="A13" s="7" t="s">
         <v>504</v>
       </c>
-      <c r="B13" s="39" t="s">
+      <c r="B13" s="38" t="s">
         <v>505</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="7"/>
-      <c r="E13" s="39" t="s">
+      <c r="E13" s="38" t="s">
         <v>506</v>
       </c>
-      <c r="F13" s="110" t="s">
+      <c r="F13" s="109" t="s">
         <v>507</v>
       </c>
     </row>
     <row r="14">
-      <c r="A14" s="99" t="s">
+      <c r="A14" s="98" t="s">
         <v>508</v>
       </c>
-      <c r="B14" s="111"/>
-      <c r="C14" s="111"/>
-      <c r="D14" s="59" t="s">
+      <c r="B14" s="110"/>
+      <c r="C14" s="110"/>
+      <c r="D14" s="58" t="s">
         <v>509</v>
       </c>
-      <c r="E14" s="39" t="s">
+      <c r="E14" s="38" t="s">
         <v>510</v>
       </c>
-      <c r="F14" s="110" t="s">
+      <c r="F14" s="109" t="s">
         <v>511</v>
       </c>
     </row>
@@ -15845,93 +15842,93 @@
   </cols>
   <sheetData>
     <row r="2">
-      <c r="A2" s="112" t="s">
+      <c r="A2" s="111" t="s">
         <v>512</v>
       </c>
-      <c r="B2" s="113" t="s">
+      <c r="B2" s="112" t="s">
         <v>513</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="114" t="s">
+      <c r="A3" s="113" t="s">
         <v>514</v>
       </c>
-      <c r="B3" s="113" t="s">
+      <c r="B3" s="112" t="s">
         <v>515</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="115" t="s">
+      <c r="A4" s="114" t="s">
         <v>516</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="116" t="s">
+      <c r="A6" s="115" t="s">
         <v>517</v>
       </c>
-      <c r="B6" s="113" t="s">
+      <c r="B6" s="112" t="s">
         <v>518</v>
       </c>
     </row>
     <row r="7">
-      <c r="B7" s="113" t="s">
+      <c r="B7" s="112" t="s">
         <v>519</v>
       </c>
     </row>
     <row r="8">
-      <c r="B8" s="113"/>
+      <c r="B8" s="112"/>
     </row>
     <row r="9">
-      <c r="B9" s="113"/>
+      <c r="B9" s="112"/>
     </row>
     <row r="10">
-      <c r="A10" s="116" t="s">
+      <c r="A10" s="115" t="s">
         <v>520</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" s="116" t="s">
+      <c r="A11" s="115" t="s">
         <v>521</v>
       </c>
-      <c r="B11" s="117" t="s">
+      <c r="B11" s="116" t="s">
         <v>522</v>
       </c>
     </row>
     <row r="12">
-      <c r="B12" s="118" t="s">
+      <c r="B12" s="117" t="s">
         <v>523</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" s="119"/>
-      <c r="B13" s="120" t="s">
+      <c r="A13" s="118"/>
+      <c r="B13" s="119" t="s">
         <v>524</v>
       </c>
     </row>
     <row r="14">
-      <c r="B14" s="121" t="s">
+      <c r="B14" s="120" t="s">
         <v>525</v>
       </c>
     </row>
     <row r="15">
-      <c r="B15" s="122" t="s">
+      <c r="B15" s="121" t="s">
         <v>526</v>
       </c>
     </row>
     <row r="16">
-      <c r="B16" s="123" t="s">
+      <c r="B16" s="122" t="s">
         <v>527</v>
       </c>
     </row>
     <row r="17">
-      <c r="A17" s="116"/>
+      <c r="A17" s="115"/>
       <c r="B17" s="28"/>
     </row>
     <row r="18">
-      <c r="A18" s="116" t="s">
+      <c r="A18" s="115" t="s">
         <v>528</v>
       </c>
-      <c r="B18" s="124" t="s">
+      <c r="B18" s="123" t="s">
         <v>529</v>
       </c>
     </row>
@@ -15939,13 +15936,13 @@
       <c r="A19" s="7" t="s">
         <v>530</v>
       </c>
-      <c r="B19" s="125"/>
+      <c r="B19" s="124"/>
     </row>
     <row r="21">
-      <c r="A21" s="116" t="s">
+      <c r="A21" s="115" t="s">
         <v>531</v>
       </c>
-      <c r="B21" s="126" t="s">
+      <c r="B21" s="125" t="s">
         <v>532</v>
       </c>
     </row>
@@ -15971,47 +15968,47 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="116" t="s">
+      <c r="A1" s="115" t="s">
         <v>533</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="127" t="s">
+      <c r="A2" s="126" t="s">
         <v>534</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="113" t="s">
+      <c r="A3" s="112" t="s">
         <v>535</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="127" t="s">
+      <c r="A4" s="126" t="s">
         <v>536</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="113" t="s">
+      <c r="A5" s="112" t="s">
         <v>537</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" s="113" t="s">
+      <c r="A6" s="112" t="s">
         <v>538</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" s="113" t="s">
+      <c r="A7" s="112" t="s">
         <v>539</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" s="127" t="s">
+      <c r="A8" s="126" t="s">
         <v>540</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="113" t="s">
+      <c r="A9" s="112" t="s">
         <v>541</v>
       </c>
     </row>
@@ -16040,12 +16037,12 @@
       <c r="A1" s="1" t="s">
         <v>533</v>
       </c>
-      <c r="B1" s="128" t="s">
+      <c r="B1" s="127" t="s">
         <v>542</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="129" t="s">
+      <c r="A2" s="128" t="s">
         <v>543</v>
       </c>
       <c r="B2" s="19" t="s">
@@ -16098,7 +16095,7 @@
   <sheetFormatPr customHeight="1" defaultColWidth="12.63" defaultRowHeight="15.75"/>
   <sheetData>
     <row r="1">
-      <c r="A1" s="117"/>
+      <c r="A1" s="116"/>
     </row>
   </sheetData>
   <drawing r:id="rId1"/>
@@ -16122,13 +16119,13 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="130" t="s">
+      <c r="A1" s="129" t="s">
         <v>551</v>
       </c>
-      <c r="C1" s="130" t="s">
+      <c r="C1" s="129" t="s">
         <v>552</v>
       </c>
-      <c r="E1" s="131" t="s">
+      <c r="E1" s="130" t="s">
         <v>2</v>
       </c>
     </row>
@@ -16148,10 +16145,10 @@
       <c r="E2" s="7"/>
     </row>
     <row r="3">
-      <c r="A3" s="36" t="s">
+      <c r="A3" s="35" t="s">
         <v>557</v>
       </c>
-      <c r="B3" s="36" t="s">
+      <c r="B3" s="35" t="s">
         <v>558</v>
       </c>
       <c r="C3" s="4" t="s">
@@ -16164,10 +16161,10 @@
       <c r="E3" s="7"/>
     </row>
     <row r="4">
-      <c r="A4" s="36" t="s">
+      <c r="A4" s="35" t="s">
         <v>560</v>
       </c>
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="35" t="s">
         <v>558</v>
       </c>
       <c r="C4" s="4" t="s">
@@ -16180,16 +16177,16 @@
       <c r="E4" s="7"/>
     </row>
     <row r="5">
-      <c r="A5" s="36" t="s">
+      <c r="A5" s="35" t="s">
         <v>561</v>
       </c>
-      <c r="B5" s="36" t="s">
+      <c r="B5" s="35" t="s">
         <v>562</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>559</v>
       </c>
-      <c r="D5" s="37" t="s">
+      <c r="D5" s="36" t="s">
         <v>563</v>
       </c>
       <c r="E5" s="7" t="s">
@@ -16248,220 +16245,220 @@
       </c>
     </row>
     <row r="9">
-      <c r="A9" s="132" t="s">
+      <c r="A9" s="131" t="s">
         <v>577</v>
       </c>
-      <c r="B9" s="133" t="s">
+      <c r="B9" s="132" t="s">
         <v>578</v>
       </c>
-      <c r="C9" s="133" t="s">
+      <c r="C9" s="132" t="s">
         <v>559</v>
       </c>
-      <c r="D9" s="133" t="s">
+      <c r="D9" s="132" t="s">
         <v>579</v>
       </c>
-      <c r="E9" s="133"/>
-      <c r="F9" s="133"/>
-      <c r="G9" s="133"/>
-      <c r="H9" s="133"/>
-      <c r="I9" s="133"/>
-      <c r="J9" s="133"/>
-      <c r="K9" s="133"/>
-      <c r="L9" s="133"/>
-      <c r="M9" s="133"/>
-      <c r="N9" s="133"/>
-      <c r="O9" s="133"/>
-      <c r="P9" s="133"/>
-      <c r="Q9" s="133"/>
-      <c r="R9" s="133"/>
-      <c r="S9" s="133"/>
-      <c r="T9" s="133"/>
-      <c r="U9" s="133"/>
-      <c r="V9" s="133"/>
-      <c r="W9" s="133"/>
-      <c r="X9" s="133"/>
-      <c r="Y9" s="133"/>
-      <c r="Z9" s="133"/>
+      <c r="E9" s="132"/>
+      <c r="F9" s="132"/>
+      <c r="G9" s="132"/>
+      <c r="H9" s="132"/>
+      <c r="I9" s="132"/>
+      <c r="J9" s="132"/>
+      <c r="K9" s="132"/>
+      <c r="L9" s="132"/>
+      <c r="M9" s="132"/>
+      <c r="N9" s="132"/>
+      <c r="O9" s="132"/>
+      <c r="P9" s="132"/>
+      <c r="Q9" s="132"/>
+      <c r="R9" s="132"/>
+      <c r="S9" s="132"/>
+      <c r="T9" s="132"/>
+      <c r="U9" s="132"/>
+      <c r="V9" s="132"/>
+      <c r="W9" s="132"/>
+      <c r="X9" s="132"/>
+      <c r="Y9" s="132"/>
+      <c r="Z9" s="132"/>
     </row>
     <row r="10">
-      <c r="A10" s="132" t="s">
+      <c r="A10" s="131" t="s">
         <v>580</v>
       </c>
-      <c r="B10" s="133" t="s">
+      <c r="B10" s="132" t="s">
         <v>578</v>
       </c>
-      <c r="C10" s="133" t="s">
+      <c r="C10" s="132" t="s">
         <v>559</v>
       </c>
-      <c r="D10" s="133" t="s">
+      <c r="D10" s="132" t="s">
         <v>581</v>
       </c>
-      <c r="E10" s="134"/>
-      <c r="F10" s="134"/>
-      <c r="G10" s="134"/>
-      <c r="H10" s="134"/>
-      <c r="I10" s="134"/>
-      <c r="J10" s="134"/>
-      <c r="K10" s="134"/>
-      <c r="L10" s="134"/>
-      <c r="M10" s="134"/>
-      <c r="N10" s="134"/>
-      <c r="O10" s="134"/>
-      <c r="P10" s="134"/>
-      <c r="Q10" s="134"/>
-      <c r="R10" s="134"/>
-      <c r="S10" s="134"/>
-      <c r="T10" s="134"/>
-      <c r="U10" s="134"/>
-      <c r="V10" s="134"/>
-      <c r="W10" s="134"/>
-      <c r="X10" s="134"/>
-      <c r="Y10" s="134"/>
-      <c r="Z10" s="134"/>
+      <c r="E10" s="133"/>
+      <c r="F10" s="133"/>
+      <c r="G10" s="133"/>
+      <c r="H10" s="133"/>
+      <c r="I10" s="133"/>
+      <c r="J10" s="133"/>
+      <c r="K10" s="133"/>
+      <c r="L10" s="133"/>
+      <c r="M10" s="133"/>
+      <c r="N10" s="133"/>
+      <c r="O10" s="133"/>
+      <c r="P10" s="133"/>
+      <c r="Q10" s="133"/>
+      <c r="R10" s="133"/>
+      <c r="S10" s="133"/>
+      <c r="T10" s="133"/>
+      <c r="U10" s="133"/>
+      <c r="V10" s="133"/>
+      <c r="W10" s="133"/>
+      <c r="X10" s="133"/>
+      <c r="Y10" s="133"/>
+      <c r="Z10" s="133"/>
     </row>
     <row r="11">
-      <c r="A11" s="132" t="s">
+      <c r="A11" s="131" t="s">
         <v>582</v>
       </c>
-      <c r="B11" s="133" t="s">
+      <c r="B11" s="132" t="s">
         <v>583</v>
       </c>
-      <c r="C11" s="133" t="s">
+      <c r="C11" s="132" t="s">
         <v>559</v>
       </c>
-      <c r="D11" s="133" t="s">
+      <c r="D11" s="132" t="s">
         <v>584</v>
       </c>
-      <c r="E11" s="134"/>
-      <c r="F11" s="134"/>
-      <c r="G11" s="134"/>
-      <c r="H11" s="134"/>
-      <c r="I11" s="134"/>
-      <c r="J11" s="134"/>
-      <c r="K11" s="134"/>
-      <c r="L11" s="134"/>
-      <c r="M11" s="134"/>
-      <c r="N11" s="134"/>
-      <c r="O11" s="134"/>
-      <c r="P11" s="134"/>
-      <c r="Q11" s="134"/>
-      <c r="R11" s="134"/>
-      <c r="S11" s="134"/>
-      <c r="T11" s="134"/>
-      <c r="U11" s="134"/>
-      <c r="V11" s="134"/>
-      <c r="W11" s="134"/>
-      <c r="X11" s="134"/>
-      <c r="Y11" s="134"/>
-      <c r="Z11" s="134"/>
+      <c r="E11" s="133"/>
+      <c r="F11" s="133"/>
+      <c r="G11" s="133"/>
+      <c r="H11" s="133"/>
+      <c r="I11" s="133"/>
+      <c r="J11" s="133"/>
+      <c r="K11" s="133"/>
+      <c r="L11" s="133"/>
+      <c r="M11" s="133"/>
+      <c r="N11" s="133"/>
+      <c r="O11" s="133"/>
+      <c r="P11" s="133"/>
+      <c r="Q11" s="133"/>
+      <c r="R11" s="133"/>
+      <c r="S11" s="133"/>
+      <c r="T11" s="133"/>
+      <c r="U11" s="133"/>
+      <c r="V11" s="133"/>
+      <c r="W11" s="133"/>
+      <c r="X11" s="133"/>
+      <c r="Y11" s="133"/>
+      <c r="Z11" s="133"/>
     </row>
     <row r="12">
-      <c r="A12" s="132" t="s">
+      <c r="A12" s="131" t="s">
         <v>585</v>
       </c>
-      <c r="B12" s="133" t="s">
+      <c r="B12" s="132" t="s">
         <v>583</v>
       </c>
-      <c r="C12" s="133" t="s">
+      <c r="C12" s="132" t="s">
         <v>559</v>
       </c>
-      <c r="D12" s="133" t="s">
+      <c r="D12" s="132" t="s">
         <v>586</v>
       </c>
-      <c r="E12" s="134"/>
-      <c r="F12" s="134"/>
-      <c r="G12" s="134"/>
-      <c r="H12" s="134"/>
-      <c r="I12" s="134"/>
-      <c r="J12" s="134"/>
-      <c r="K12" s="134"/>
-      <c r="L12" s="134"/>
-      <c r="M12" s="134"/>
-      <c r="N12" s="134"/>
-      <c r="O12" s="134"/>
-      <c r="P12" s="134"/>
-      <c r="Q12" s="134"/>
-      <c r="R12" s="134"/>
-      <c r="S12" s="134"/>
-      <c r="T12" s="134"/>
-      <c r="U12" s="134"/>
-      <c r="V12" s="134"/>
-      <c r="W12" s="134"/>
-      <c r="X12" s="134"/>
-      <c r="Y12" s="134"/>
-      <c r="Z12" s="134"/>
+      <c r="E12" s="133"/>
+      <c r="F12" s="133"/>
+      <c r="G12" s="133"/>
+      <c r="H12" s="133"/>
+      <c r="I12" s="133"/>
+      <c r="J12" s="133"/>
+      <c r="K12" s="133"/>
+      <c r="L12" s="133"/>
+      <c r="M12" s="133"/>
+      <c r="N12" s="133"/>
+      <c r="O12" s="133"/>
+      <c r="P12" s="133"/>
+      <c r="Q12" s="133"/>
+      <c r="R12" s="133"/>
+      <c r="S12" s="133"/>
+      <c r="T12" s="133"/>
+      <c r="U12" s="133"/>
+      <c r="V12" s="133"/>
+      <c r="W12" s="133"/>
+      <c r="X12" s="133"/>
+      <c r="Y12" s="133"/>
+      <c r="Z12" s="133"/>
     </row>
     <row r="13">
-      <c r="A13" s="132" t="s">
+      <c r="A13" s="131" t="s">
         <v>587</v>
       </c>
-      <c r="B13" s="132" t="s">
+      <c r="B13" s="131" t="s">
         <v>562</v>
       </c>
-      <c r="C13" s="133" t="s">
+      <c r="C13" s="132" t="s">
         <v>559</v>
       </c>
-      <c r="D13" s="133" t="s">
+      <c r="D13" s="132" t="s">
         <v>588</v>
       </c>
-      <c r="E13" s="134"/>
-      <c r="F13" s="134"/>
-      <c r="G13" s="134"/>
-      <c r="H13" s="134"/>
-      <c r="I13" s="134"/>
-      <c r="J13" s="134"/>
-      <c r="K13" s="134"/>
-      <c r="L13" s="134"/>
-      <c r="M13" s="134"/>
-      <c r="N13" s="134"/>
-      <c r="O13" s="134"/>
-      <c r="P13" s="134"/>
-      <c r="Q13" s="134"/>
-      <c r="R13" s="134"/>
-      <c r="S13" s="134"/>
-      <c r="T13" s="134"/>
-      <c r="U13" s="134"/>
-      <c r="V13" s="134"/>
-      <c r="W13" s="134"/>
-      <c r="X13" s="134"/>
-      <c r="Y13" s="134"/>
-      <c r="Z13" s="134"/>
+      <c r="E13" s="133"/>
+      <c r="F13" s="133"/>
+      <c r="G13" s="133"/>
+      <c r="H13" s="133"/>
+      <c r="I13" s="133"/>
+      <c r="J13" s="133"/>
+      <c r="K13" s="133"/>
+      <c r="L13" s="133"/>
+      <c r="M13" s="133"/>
+      <c r="N13" s="133"/>
+      <c r="O13" s="133"/>
+      <c r="P13" s="133"/>
+      <c r="Q13" s="133"/>
+      <c r="R13" s="133"/>
+      <c r="S13" s="133"/>
+      <c r="T13" s="133"/>
+      <c r="U13" s="133"/>
+      <c r="V13" s="133"/>
+      <c r="W13" s="133"/>
+      <c r="X13" s="133"/>
+      <c r="Y13" s="133"/>
+      <c r="Z13" s="133"/>
     </row>
     <row r="14">
-      <c r="A14" s="132" t="s">
+      <c r="A14" s="131" t="s">
         <v>589</v>
       </c>
-      <c r="B14" s="132" t="s">
+      <c r="B14" s="131" t="s">
         <v>562</v>
       </c>
-      <c r="C14" s="133" t="s">
+      <c r="C14" s="132" t="s">
         <v>559</v>
       </c>
-      <c r="D14" s="133" t="s">
+      <c r="D14" s="132" t="s">
         <v>590</v>
       </c>
-      <c r="E14" s="134"/>
-      <c r="F14" s="134"/>
-      <c r="G14" s="134"/>
-      <c r="H14" s="134"/>
-      <c r="I14" s="134"/>
-      <c r="J14" s="134"/>
-      <c r="K14" s="134"/>
-      <c r="L14" s="134"/>
-      <c r="M14" s="134"/>
-      <c r="N14" s="134"/>
-      <c r="O14" s="134"/>
-      <c r="P14" s="134"/>
-      <c r="Q14" s="134"/>
-      <c r="R14" s="134"/>
-      <c r="S14" s="134"/>
-      <c r="T14" s="134"/>
-      <c r="U14" s="134"/>
-      <c r="V14" s="134"/>
-      <c r="W14" s="134"/>
-      <c r="X14" s="134"/>
-      <c r="Y14" s="134"/>
-      <c r="Z14" s="134"/>
+      <c r="E14" s="133"/>
+      <c r="F14" s="133"/>
+      <c r="G14" s="133"/>
+      <c r="H14" s="133"/>
+      <c r="I14" s="133"/>
+      <c r="J14" s="133"/>
+      <c r="K14" s="133"/>
+      <c r="L14" s="133"/>
+      <c r="M14" s="133"/>
+      <c r="N14" s="133"/>
+      <c r="O14" s="133"/>
+      <c r="P14" s="133"/>
+      <c r="Q14" s="133"/>
+      <c r="R14" s="133"/>
+      <c r="S14" s="133"/>
+      <c r="T14" s="133"/>
+      <c r="U14" s="133"/>
+      <c r="V14" s="133"/>
+      <c r="W14" s="133"/>
+      <c r="X14" s="133"/>
+      <c r="Y14" s="133"/>
+      <c r="Z14" s="133"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -16489,51 +16486,51 @@
   </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" s="135" t="s">
+      <c r="A1" s="134" t="s">
         <v>551</v>
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="116" t="s">
+      <c r="A2" s="115" t="s">
         <v>553</v>
       </c>
-      <c r="B2" s="116" t="s">
+      <c r="B2" s="115" t="s">
         <v>554</v>
       </c>
-      <c r="C2" s="116" t="s">
+      <c r="C2" s="115" t="s">
         <v>555</v>
       </c>
-      <c r="D2" s="116" t="s">
+      <c r="D2" s="115" t="s">
         <v>556</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" s="113" t="s">
+      <c r="A3" s="112" t="s">
         <v>591</v>
       </c>
-      <c r="B3" s="113" t="s">
+      <c r="B3" s="112" t="s">
         <v>592</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" s="113" t="s">
+      <c r="A4" s="112" t="s">
         <v>593</v>
       </c>
-      <c r="B4" s="113" t="s">
+      <c r="B4" s="112" t="s">
         <v>594</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" s="113" t="s">
+      <c r="A5" s="112" t="s">
         <v>595</v>
       </c>
-      <c r="B5" s="113" t="s">
+      <c r="B5" s="112" t="s">
         <v>596</v>
       </c>
-      <c r="C5" s="136" t="s">
+      <c r="C5" s="135" t="s">
         <v>594</v>
       </c>
-      <c r="D5" s="113" t="s">
+      <c r="D5" s="112" t="s">
         <v>597</v>
       </c>
     </row>

</xml_diff>